<commit_message>
Added Robot Return to Origin practice
</commit_message>
<xml_diff>
--- a/LeetCode_Results.xlsx
+++ b/LeetCode_Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>LeetCode Practice Results</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Flipping an Image</t>
+  </si>
+  <si>
+    <t>Robot Return to Origin</t>
   </si>
 </sst>
 </file>
@@ -615,7 +618,7 @@
   <dimension ref="A1:Z409"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19:Q19"/>
+      <selection activeCell="A20" sqref="A20:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,7 +768,7 @@
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="str">
         <f>"Average Results: " &amp; SUM(K10:M500) &amp; " submitted C# answers are faster than "  &amp; ROUNDDOWN(AVERAGE(N10:O500), 2) &amp; "% and has a lesser memory usage by " &amp; ROUNDDOWN(AVERAGE(P10:Q500), 2) &amp; "% out of all C# submissions."</f>
-        <v>Average Results: 10 submitted C# answers are faster than 92.83% and has a lesser memory usage by 51.85% out of all C# submissions.</v>
+        <v>Average Results: 11 submitted C# answers are faster than 92.8% and has a lesser memory usage by 48.65% out of all C# submissions.</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -1147,7 +1150,9 @@
       <c r="Q19" s="2"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1157,12 +1162,18 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="2"/>
+      <c r="K20" s="2">
+        <v>1</v>
+      </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
-      <c r="N20" s="1"/>
+      <c r="N20" s="1">
+        <v>92.56</v>
+      </c>
       <c r="O20" s="1"/>
-      <c r="P20" s="2"/>
+      <c r="P20" s="2">
+        <v>16.670000000000002</v>
+      </c>
       <c r="Q20" s="2"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -8558,28 +8569,1566 @@
     </row>
   </sheetData>
   <mergeCells count="1606">
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="A10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="A1:Z5"/>
-    <mergeCell ref="A6:Z8"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="A408:J408"/>
+    <mergeCell ref="K408:M408"/>
+    <mergeCell ref="N408:O408"/>
+    <mergeCell ref="P408:Q408"/>
+    <mergeCell ref="A409:J409"/>
+    <mergeCell ref="K409:M409"/>
+    <mergeCell ref="N409:O409"/>
+    <mergeCell ref="P409:Q409"/>
+    <mergeCell ref="A406:J406"/>
+    <mergeCell ref="K406:M406"/>
+    <mergeCell ref="N406:O406"/>
+    <mergeCell ref="P406:Q406"/>
+    <mergeCell ref="A407:J407"/>
+    <mergeCell ref="K407:M407"/>
+    <mergeCell ref="N407:O407"/>
+    <mergeCell ref="P407:Q407"/>
+    <mergeCell ref="A404:J404"/>
+    <mergeCell ref="K404:M404"/>
+    <mergeCell ref="N404:O404"/>
+    <mergeCell ref="P404:Q404"/>
+    <mergeCell ref="A405:J405"/>
+    <mergeCell ref="K405:M405"/>
+    <mergeCell ref="N405:O405"/>
+    <mergeCell ref="P405:Q405"/>
+    <mergeCell ref="A402:J402"/>
+    <mergeCell ref="K402:M402"/>
+    <mergeCell ref="N402:O402"/>
+    <mergeCell ref="P402:Q402"/>
+    <mergeCell ref="A403:J403"/>
+    <mergeCell ref="K403:M403"/>
+    <mergeCell ref="N403:O403"/>
+    <mergeCell ref="P403:Q403"/>
+    <mergeCell ref="A400:J400"/>
+    <mergeCell ref="K400:M400"/>
+    <mergeCell ref="N400:O400"/>
+    <mergeCell ref="P400:Q400"/>
+    <mergeCell ref="A401:J401"/>
+    <mergeCell ref="K401:M401"/>
+    <mergeCell ref="N401:O401"/>
+    <mergeCell ref="P401:Q401"/>
+    <mergeCell ref="A398:J398"/>
+    <mergeCell ref="K398:M398"/>
+    <mergeCell ref="N398:O398"/>
+    <mergeCell ref="P398:Q398"/>
+    <mergeCell ref="A399:J399"/>
+    <mergeCell ref="K399:M399"/>
+    <mergeCell ref="N399:O399"/>
+    <mergeCell ref="P399:Q399"/>
+    <mergeCell ref="A396:J396"/>
+    <mergeCell ref="K396:M396"/>
+    <mergeCell ref="N396:O396"/>
+    <mergeCell ref="P396:Q396"/>
+    <mergeCell ref="A397:J397"/>
+    <mergeCell ref="K397:M397"/>
+    <mergeCell ref="N397:O397"/>
+    <mergeCell ref="P397:Q397"/>
+    <mergeCell ref="A394:J394"/>
+    <mergeCell ref="K394:M394"/>
+    <mergeCell ref="N394:O394"/>
+    <mergeCell ref="P394:Q394"/>
+    <mergeCell ref="A395:J395"/>
+    <mergeCell ref="K395:M395"/>
+    <mergeCell ref="N395:O395"/>
+    <mergeCell ref="P395:Q395"/>
+    <mergeCell ref="A392:J392"/>
+    <mergeCell ref="K392:M392"/>
+    <mergeCell ref="N392:O392"/>
+    <mergeCell ref="P392:Q392"/>
+    <mergeCell ref="A393:J393"/>
+    <mergeCell ref="K393:M393"/>
+    <mergeCell ref="N393:O393"/>
+    <mergeCell ref="P393:Q393"/>
+    <mergeCell ref="A390:J390"/>
+    <mergeCell ref="K390:M390"/>
+    <mergeCell ref="N390:O390"/>
+    <mergeCell ref="P390:Q390"/>
+    <mergeCell ref="A391:J391"/>
+    <mergeCell ref="K391:M391"/>
+    <mergeCell ref="N391:O391"/>
+    <mergeCell ref="P391:Q391"/>
+    <mergeCell ref="A388:J388"/>
+    <mergeCell ref="K388:M388"/>
+    <mergeCell ref="N388:O388"/>
+    <mergeCell ref="P388:Q388"/>
+    <mergeCell ref="A389:J389"/>
+    <mergeCell ref="K389:M389"/>
+    <mergeCell ref="N389:O389"/>
+    <mergeCell ref="P389:Q389"/>
+    <mergeCell ref="A386:J386"/>
+    <mergeCell ref="K386:M386"/>
+    <mergeCell ref="N386:O386"/>
+    <mergeCell ref="P386:Q386"/>
+    <mergeCell ref="A387:J387"/>
+    <mergeCell ref="K387:M387"/>
+    <mergeCell ref="N387:O387"/>
+    <mergeCell ref="P387:Q387"/>
+    <mergeCell ref="A384:J384"/>
+    <mergeCell ref="K384:M384"/>
+    <mergeCell ref="N384:O384"/>
+    <mergeCell ref="P384:Q384"/>
+    <mergeCell ref="A385:J385"/>
+    <mergeCell ref="K385:M385"/>
+    <mergeCell ref="N385:O385"/>
+    <mergeCell ref="P385:Q385"/>
+    <mergeCell ref="A382:J382"/>
+    <mergeCell ref="K382:M382"/>
+    <mergeCell ref="N382:O382"/>
+    <mergeCell ref="P382:Q382"/>
+    <mergeCell ref="A383:J383"/>
+    <mergeCell ref="K383:M383"/>
+    <mergeCell ref="N383:O383"/>
+    <mergeCell ref="P383:Q383"/>
+    <mergeCell ref="A380:J380"/>
+    <mergeCell ref="K380:M380"/>
+    <mergeCell ref="N380:O380"/>
+    <mergeCell ref="P380:Q380"/>
+    <mergeCell ref="A381:J381"/>
+    <mergeCell ref="K381:M381"/>
+    <mergeCell ref="N381:O381"/>
+    <mergeCell ref="P381:Q381"/>
+    <mergeCell ref="A378:J378"/>
+    <mergeCell ref="K378:M378"/>
+    <mergeCell ref="N378:O378"/>
+    <mergeCell ref="P378:Q378"/>
+    <mergeCell ref="A379:J379"/>
+    <mergeCell ref="K379:M379"/>
+    <mergeCell ref="N379:O379"/>
+    <mergeCell ref="P379:Q379"/>
+    <mergeCell ref="A376:J376"/>
+    <mergeCell ref="K376:M376"/>
+    <mergeCell ref="N376:O376"/>
+    <mergeCell ref="P376:Q376"/>
+    <mergeCell ref="A377:J377"/>
+    <mergeCell ref="K377:M377"/>
+    <mergeCell ref="N377:O377"/>
+    <mergeCell ref="P377:Q377"/>
+    <mergeCell ref="A374:J374"/>
+    <mergeCell ref="K374:M374"/>
+    <mergeCell ref="N374:O374"/>
+    <mergeCell ref="P374:Q374"/>
+    <mergeCell ref="A375:J375"/>
+    <mergeCell ref="K375:M375"/>
+    <mergeCell ref="N375:O375"/>
+    <mergeCell ref="P375:Q375"/>
+    <mergeCell ref="A372:J372"/>
+    <mergeCell ref="K372:M372"/>
+    <mergeCell ref="N372:O372"/>
+    <mergeCell ref="P372:Q372"/>
+    <mergeCell ref="A373:J373"/>
+    <mergeCell ref="K373:M373"/>
+    <mergeCell ref="N373:O373"/>
+    <mergeCell ref="P373:Q373"/>
+    <mergeCell ref="A370:J370"/>
+    <mergeCell ref="K370:M370"/>
+    <mergeCell ref="N370:O370"/>
+    <mergeCell ref="P370:Q370"/>
+    <mergeCell ref="A371:J371"/>
+    <mergeCell ref="K371:M371"/>
+    <mergeCell ref="N371:O371"/>
+    <mergeCell ref="P371:Q371"/>
+    <mergeCell ref="A368:J368"/>
+    <mergeCell ref="K368:M368"/>
+    <mergeCell ref="N368:O368"/>
+    <mergeCell ref="P368:Q368"/>
+    <mergeCell ref="A369:J369"/>
+    <mergeCell ref="K369:M369"/>
+    <mergeCell ref="N369:O369"/>
+    <mergeCell ref="P369:Q369"/>
+    <mergeCell ref="A366:J366"/>
+    <mergeCell ref="K366:M366"/>
+    <mergeCell ref="N366:O366"/>
+    <mergeCell ref="P366:Q366"/>
+    <mergeCell ref="A367:J367"/>
+    <mergeCell ref="K367:M367"/>
+    <mergeCell ref="N367:O367"/>
+    <mergeCell ref="P367:Q367"/>
+    <mergeCell ref="A364:J364"/>
+    <mergeCell ref="K364:M364"/>
+    <mergeCell ref="N364:O364"/>
+    <mergeCell ref="P364:Q364"/>
+    <mergeCell ref="A365:J365"/>
+    <mergeCell ref="K365:M365"/>
+    <mergeCell ref="N365:O365"/>
+    <mergeCell ref="P365:Q365"/>
+    <mergeCell ref="A362:J362"/>
+    <mergeCell ref="K362:M362"/>
+    <mergeCell ref="N362:O362"/>
+    <mergeCell ref="P362:Q362"/>
+    <mergeCell ref="A363:J363"/>
+    <mergeCell ref="K363:M363"/>
+    <mergeCell ref="N363:O363"/>
+    <mergeCell ref="P363:Q363"/>
+    <mergeCell ref="A360:J360"/>
+    <mergeCell ref="K360:M360"/>
+    <mergeCell ref="N360:O360"/>
+    <mergeCell ref="P360:Q360"/>
+    <mergeCell ref="A361:J361"/>
+    <mergeCell ref="K361:M361"/>
+    <mergeCell ref="N361:O361"/>
+    <mergeCell ref="P361:Q361"/>
+    <mergeCell ref="A358:J358"/>
+    <mergeCell ref="K358:M358"/>
+    <mergeCell ref="N358:O358"/>
+    <mergeCell ref="P358:Q358"/>
+    <mergeCell ref="A359:J359"/>
+    <mergeCell ref="K359:M359"/>
+    <mergeCell ref="N359:O359"/>
+    <mergeCell ref="P359:Q359"/>
+    <mergeCell ref="A356:J356"/>
+    <mergeCell ref="K356:M356"/>
+    <mergeCell ref="N356:O356"/>
+    <mergeCell ref="P356:Q356"/>
+    <mergeCell ref="A357:J357"/>
+    <mergeCell ref="K357:M357"/>
+    <mergeCell ref="N357:O357"/>
+    <mergeCell ref="P357:Q357"/>
+    <mergeCell ref="A354:J354"/>
+    <mergeCell ref="K354:M354"/>
+    <mergeCell ref="N354:O354"/>
+    <mergeCell ref="P354:Q354"/>
+    <mergeCell ref="A355:J355"/>
+    <mergeCell ref="K355:M355"/>
+    <mergeCell ref="N355:O355"/>
+    <mergeCell ref="P355:Q355"/>
+    <mergeCell ref="A352:J352"/>
+    <mergeCell ref="K352:M352"/>
+    <mergeCell ref="N352:O352"/>
+    <mergeCell ref="P352:Q352"/>
+    <mergeCell ref="A353:J353"/>
+    <mergeCell ref="K353:M353"/>
+    <mergeCell ref="N353:O353"/>
+    <mergeCell ref="P353:Q353"/>
+    <mergeCell ref="A350:J350"/>
+    <mergeCell ref="K350:M350"/>
+    <mergeCell ref="N350:O350"/>
+    <mergeCell ref="P350:Q350"/>
+    <mergeCell ref="A351:J351"/>
+    <mergeCell ref="K351:M351"/>
+    <mergeCell ref="N351:O351"/>
+    <mergeCell ref="P351:Q351"/>
+    <mergeCell ref="A348:J348"/>
+    <mergeCell ref="K348:M348"/>
+    <mergeCell ref="N348:O348"/>
+    <mergeCell ref="P348:Q348"/>
+    <mergeCell ref="A349:J349"/>
+    <mergeCell ref="K349:M349"/>
+    <mergeCell ref="N349:O349"/>
+    <mergeCell ref="P349:Q349"/>
+    <mergeCell ref="A346:J346"/>
+    <mergeCell ref="K346:M346"/>
+    <mergeCell ref="N346:O346"/>
+    <mergeCell ref="P346:Q346"/>
+    <mergeCell ref="A347:J347"/>
+    <mergeCell ref="K347:M347"/>
+    <mergeCell ref="N347:O347"/>
+    <mergeCell ref="P347:Q347"/>
+    <mergeCell ref="A344:J344"/>
+    <mergeCell ref="K344:M344"/>
+    <mergeCell ref="N344:O344"/>
+    <mergeCell ref="P344:Q344"/>
+    <mergeCell ref="A345:J345"/>
+    <mergeCell ref="K345:M345"/>
+    <mergeCell ref="N345:O345"/>
+    <mergeCell ref="P345:Q345"/>
+    <mergeCell ref="A342:J342"/>
+    <mergeCell ref="K342:M342"/>
+    <mergeCell ref="N342:O342"/>
+    <mergeCell ref="P342:Q342"/>
+    <mergeCell ref="A343:J343"/>
+    <mergeCell ref="K343:M343"/>
+    <mergeCell ref="N343:O343"/>
+    <mergeCell ref="P343:Q343"/>
+    <mergeCell ref="A340:J340"/>
+    <mergeCell ref="K340:M340"/>
+    <mergeCell ref="N340:O340"/>
+    <mergeCell ref="P340:Q340"/>
+    <mergeCell ref="A341:J341"/>
+    <mergeCell ref="K341:M341"/>
+    <mergeCell ref="N341:O341"/>
+    <mergeCell ref="P341:Q341"/>
+    <mergeCell ref="A338:J338"/>
+    <mergeCell ref="K338:M338"/>
+    <mergeCell ref="N338:O338"/>
+    <mergeCell ref="P338:Q338"/>
+    <mergeCell ref="A339:J339"/>
+    <mergeCell ref="K339:M339"/>
+    <mergeCell ref="N339:O339"/>
+    <mergeCell ref="P339:Q339"/>
+    <mergeCell ref="A336:J336"/>
+    <mergeCell ref="K336:M336"/>
+    <mergeCell ref="N336:O336"/>
+    <mergeCell ref="P336:Q336"/>
+    <mergeCell ref="A337:J337"/>
+    <mergeCell ref="K337:M337"/>
+    <mergeCell ref="N337:O337"/>
+    <mergeCell ref="P337:Q337"/>
+    <mergeCell ref="A334:J334"/>
+    <mergeCell ref="K334:M334"/>
+    <mergeCell ref="N334:O334"/>
+    <mergeCell ref="P334:Q334"/>
+    <mergeCell ref="A335:J335"/>
+    <mergeCell ref="K335:M335"/>
+    <mergeCell ref="N335:O335"/>
+    <mergeCell ref="P335:Q335"/>
+    <mergeCell ref="A332:J332"/>
+    <mergeCell ref="K332:M332"/>
+    <mergeCell ref="N332:O332"/>
+    <mergeCell ref="P332:Q332"/>
+    <mergeCell ref="A333:J333"/>
+    <mergeCell ref="K333:M333"/>
+    <mergeCell ref="N333:O333"/>
+    <mergeCell ref="P333:Q333"/>
+    <mergeCell ref="A330:J330"/>
+    <mergeCell ref="K330:M330"/>
+    <mergeCell ref="N330:O330"/>
+    <mergeCell ref="P330:Q330"/>
+    <mergeCell ref="A331:J331"/>
+    <mergeCell ref="K331:M331"/>
+    <mergeCell ref="N331:O331"/>
+    <mergeCell ref="P331:Q331"/>
+    <mergeCell ref="A328:J328"/>
+    <mergeCell ref="K328:M328"/>
+    <mergeCell ref="N328:O328"/>
+    <mergeCell ref="P328:Q328"/>
+    <mergeCell ref="A329:J329"/>
+    <mergeCell ref="K329:M329"/>
+    <mergeCell ref="N329:O329"/>
+    <mergeCell ref="P329:Q329"/>
+    <mergeCell ref="A326:J326"/>
+    <mergeCell ref="K326:M326"/>
+    <mergeCell ref="N326:O326"/>
+    <mergeCell ref="P326:Q326"/>
+    <mergeCell ref="A327:J327"/>
+    <mergeCell ref="K327:M327"/>
+    <mergeCell ref="N327:O327"/>
+    <mergeCell ref="P327:Q327"/>
+    <mergeCell ref="A324:J324"/>
+    <mergeCell ref="K324:M324"/>
+    <mergeCell ref="N324:O324"/>
+    <mergeCell ref="P324:Q324"/>
+    <mergeCell ref="A325:J325"/>
+    <mergeCell ref="K325:M325"/>
+    <mergeCell ref="N325:O325"/>
+    <mergeCell ref="P325:Q325"/>
+    <mergeCell ref="A322:J322"/>
+    <mergeCell ref="K322:M322"/>
+    <mergeCell ref="N322:O322"/>
+    <mergeCell ref="P322:Q322"/>
+    <mergeCell ref="A323:J323"/>
+    <mergeCell ref="K323:M323"/>
+    <mergeCell ref="N323:O323"/>
+    <mergeCell ref="P323:Q323"/>
+    <mergeCell ref="A320:J320"/>
+    <mergeCell ref="K320:M320"/>
+    <mergeCell ref="N320:O320"/>
+    <mergeCell ref="P320:Q320"/>
+    <mergeCell ref="A321:J321"/>
+    <mergeCell ref="K321:M321"/>
+    <mergeCell ref="N321:O321"/>
+    <mergeCell ref="P321:Q321"/>
+    <mergeCell ref="A318:J318"/>
+    <mergeCell ref="K318:M318"/>
+    <mergeCell ref="N318:O318"/>
+    <mergeCell ref="P318:Q318"/>
+    <mergeCell ref="A319:J319"/>
+    <mergeCell ref="K319:M319"/>
+    <mergeCell ref="N319:O319"/>
+    <mergeCell ref="P319:Q319"/>
+    <mergeCell ref="A316:J316"/>
+    <mergeCell ref="K316:M316"/>
+    <mergeCell ref="N316:O316"/>
+    <mergeCell ref="P316:Q316"/>
+    <mergeCell ref="A317:J317"/>
+    <mergeCell ref="K317:M317"/>
+    <mergeCell ref="N317:O317"/>
+    <mergeCell ref="P317:Q317"/>
+    <mergeCell ref="A314:J314"/>
+    <mergeCell ref="K314:M314"/>
+    <mergeCell ref="N314:O314"/>
+    <mergeCell ref="P314:Q314"/>
+    <mergeCell ref="A315:J315"/>
+    <mergeCell ref="K315:M315"/>
+    <mergeCell ref="N315:O315"/>
+    <mergeCell ref="P315:Q315"/>
+    <mergeCell ref="A312:J312"/>
+    <mergeCell ref="K312:M312"/>
+    <mergeCell ref="N312:O312"/>
+    <mergeCell ref="P312:Q312"/>
+    <mergeCell ref="A313:J313"/>
+    <mergeCell ref="K313:M313"/>
+    <mergeCell ref="N313:O313"/>
+    <mergeCell ref="P313:Q313"/>
+    <mergeCell ref="A310:J310"/>
+    <mergeCell ref="K310:M310"/>
+    <mergeCell ref="N310:O310"/>
+    <mergeCell ref="P310:Q310"/>
+    <mergeCell ref="A311:J311"/>
+    <mergeCell ref="K311:M311"/>
+    <mergeCell ref="N311:O311"/>
+    <mergeCell ref="P311:Q311"/>
+    <mergeCell ref="A308:J308"/>
+    <mergeCell ref="K308:M308"/>
+    <mergeCell ref="N308:O308"/>
+    <mergeCell ref="P308:Q308"/>
+    <mergeCell ref="A309:J309"/>
+    <mergeCell ref="K309:M309"/>
+    <mergeCell ref="N309:O309"/>
+    <mergeCell ref="P309:Q309"/>
+    <mergeCell ref="A306:J306"/>
+    <mergeCell ref="K306:M306"/>
+    <mergeCell ref="N306:O306"/>
+    <mergeCell ref="P306:Q306"/>
+    <mergeCell ref="A307:J307"/>
+    <mergeCell ref="K307:M307"/>
+    <mergeCell ref="N307:O307"/>
+    <mergeCell ref="P307:Q307"/>
+    <mergeCell ref="A304:J304"/>
+    <mergeCell ref="K304:M304"/>
+    <mergeCell ref="N304:O304"/>
+    <mergeCell ref="P304:Q304"/>
+    <mergeCell ref="A305:J305"/>
+    <mergeCell ref="K305:M305"/>
+    <mergeCell ref="N305:O305"/>
+    <mergeCell ref="P305:Q305"/>
+    <mergeCell ref="A302:J302"/>
+    <mergeCell ref="K302:M302"/>
+    <mergeCell ref="N302:O302"/>
+    <mergeCell ref="P302:Q302"/>
+    <mergeCell ref="A303:J303"/>
+    <mergeCell ref="K303:M303"/>
+    <mergeCell ref="N303:O303"/>
+    <mergeCell ref="P303:Q303"/>
+    <mergeCell ref="A300:J300"/>
+    <mergeCell ref="K300:M300"/>
+    <mergeCell ref="N300:O300"/>
+    <mergeCell ref="P300:Q300"/>
+    <mergeCell ref="A301:J301"/>
+    <mergeCell ref="K301:M301"/>
+    <mergeCell ref="N301:O301"/>
+    <mergeCell ref="P301:Q301"/>
+    <mergeCell ref="A298:J298"/>
+    <mergeCell ref="K298:M298"/>
+    <mergeCell ref="N298:O298"/>
+    <mergeCell ref="P298:Q298"/>
+    <mergeCell ref="A299:J299"/>
+    <mergeCell ref="K299:M299"/>
+    <mergeCell ref="N299:O299"/>
+    <mergeCell ref="P299:Q299"/>
+    <mergeCell ref="A296:J296"/>
+    <mergeCell ref="K296:M296"/>
+    <mergeCell ref="N296:O296"/>
+    <mergeCell ref="P296:Q296"/>
+    <mergeCell ref="A297:J297"/>
+    <mergeCell ref="K297:M297"/>
+    <mergeCell ref="N297:O297"/>
+    <mergeCell ref="P297:Q297"/>
+    <mergeCell ref="A294:J294"/>
+    <mergeCell ref="K294:M294"/>
+    <mergeCell ref="N294:O294"/>
+    <mergeCell ref="P294:Q294"/>
+    <mergeCell ref="A295:J295"/>
+    <mergeCell ref="K295:M295"/>
+    <mergeCell ref="N295:O295"/>
+    <mergeCell ref="P295:Q295"/>
+    <mergeCell ref="A292:J292"/>
+    <mergeCell ref="K292:M292"/>
+    <mergeCell ref="N292:O292"/>
+    <mergeCell ref="P292:Q292"/>
+    <mergeCell ref="A293:J293"/>
+    <mergeCell ref="K293:M293"/>
+    <mergeCell ref="N293:O293"/>
+    <mergeCell ref="P293:Q293"/>
+    <mergeCell ref="A290:J290"/>
+    <mergeCell ref="K290:M290"/>
+    <mergeCell ref="N290:O290"/>
+    <mergeCell ref="P290:Q290"/>
+    <mergeCell ref="A291:J291"/>
+    <mergeCell ref="K291:M291"/>
+    <mergeCell ref="N291:O291"/>
+    <mergeCell ref="P291:Q291"/>
+    <mergeCell ref="A288:J288"/>
+    <mergeCell ref="K288:M288"/>
+    <mergeCell ref="N288:O288"/>
+    <mergeCell ref="P288:Q288"/>
+    <mergeCell ref="A289:J289"/>
+    <mergeCell ref="K289:M289"/>
+    <mergeCell ref="N289:O289"/>
+    <mergeCell ref="P289:Q289"/>
+    <mergeCell ref="A286:J286"/>
+    <mergeCell ref="K286:M286"/>
+    <mergeCell ref="N286:O286"/>
+    <mergeCell ref="P286:Q286"/>
+    <mergeCell ref="A287:J287"/>
+    <mergeCell ref="K287:M287"/>
+    <mergeCell ref="N287:O287"/>
+    <mergeCell ref="P287:Q287"/>
+    <mergeCell ref="A284:J284"/>
+    <mergeCell ref="K284:M284"/>
+    <mergeCell ref="N284:O284"/>
+    <mergeCell ref="P284:Q284"/>
+    <mergeCell ref="A285:J285"/>
+    <mergeCell ref="K285:M285"/>
+    <mergeCell ref="N285:O285"/>
+    <mergeCell ref="P285:Q285"/>
+    <mergeCell ref="A282:J282"/>
+    <mergeCell ref="K282:M282"/>
+    <mergeCell ref="N282:O282"/>
+    <mergeCell ref="P282:Q282"/>
+    <mergeCell ref="A283:J283"/>
+    <mergeCell ref="K283:M283"/>
+    <mergeCell ref="N283:O283"/>
+    <mergeCell ref="P283:Q283"/>
+    <mergeCell ref="A280:J280"/>
+    <mergeCell ref="K280:M280"/>
+    <mergeCell ref="N280:O280"/>
+    <mergeCell ref="P280:Q280"/>
+    <mergeCell ref="A281:J281"/>
+    <mergeCell ref="K281:M281"/>
+    <mergeCell ref="N281:O281"/>
+    <mergeCell ref="P281:Q281"/>
+    <mergeCell ref="A278:J278"/>
+    <mergeCell ref="K278:M278"/>
+    <mergeCell ref="N278:O278"/>
+    <mergeCell ref="P278:Q278"/>
+    <mergeCell ref="A279:J279"/>
+    <mergeCell ref="K279:M279"/>
+    <mergeCell ref="N279:O279"/>
+    <mergeCell ref="P279:Q279"/>
+    <mergeCell ref="A276:J276"/>
+    <mergeCell ref="K276:M276"/>
+    <mergeCell ref="N276:O276"/>
+    <mergeCell ref="P276:Q276"/>
+    <mergeCell ref="A277:J277"/>
+    <mergeCell ref="K277:M277"/>
+    <mergeCell ref="N277:O277"/>
+    <mergeCell ref="P277:Q277"/>
+    <mergeCell ref="A274:J274"/>
+    <mergeCell ref="K274:M274"/>
+    <mergeCell ref="N274:O274"/>
+    <mergeCell ref="P274:Q274"/>
+    <mergeCell ref="A275:J275"/>
+    <mergeCell ref="K275:M275"/>
+    <mergeCell ref="N275:O275"/>
+    <mergeCell ref="P275:Q275"/>
+    <mergeCell ref="A272:J272"/>
+    <mergeCell ref="K272:M272"/>
+    <mergeCell ref="N272:O272"/>
+    <mergeCell ref="P272:Q272"/>
+    <mergeCell ref="A273:J273"/>
+    <mergeCell ref="K273:M273"/>
+    <mergeCell ref="N273:O273"/>
+    <mergeCell ref="P273:Q273"/>
+    <mergeCell ref="A270:J270"/>
+    <mergeCell ref="K270:M270"/>
+    <mergeCell ref="N270:O270"/>
+    <mergeCell ref="P270:Q270"/>
+    <mergeCell ref="A271:J271"/>
+    <mergeCell ref="K271:M271"/>
+    <mergeCell ref="N271:O271"/>
+    <mergeCell ref="P271:Q271"/>
+    <mergeCell ref="A268:J268"/>
+    <mergeCell ref="K268:M268"/>
+    <mergeCell ref="N268:O268"/>
+    <mergeCell ref="P268:Q268"/>
+    <mergeCell ref="A269:J269"/>
+    <mergeCell ref="K269:M269"/>
+    <mergeCell ref="N269:O269"/>
+    <mergeCell ref="P269:Q269"/>
+    <mergeCell ref="A266:J266"/>
+    <mergeCell ref="K266:M266"/>
+    <mergeCell ref="N266:O266"/>
+    <mergeCell ref="P266:Q266"/>
+    <mergeCell ref="A267:J267"/>
+    <mergeCell ref="K267:M267"/>
+    <mergeCell ref="N267:O267"/>
+    <mergeCell ref="P267:Q267"/>
+    <mergeCell ref="A264:J264"/>
+    <mergeCell ref="K264:M264"/>
+    <mergeCell ref="N264:O264"/>
+    <mergeCell ref="P264:Q264"/>
+    <mergeCell ref="A265:J265"/>
+    <mergeCell ref="K265:M265"/>
+    <mergeCell ref="N265:O265"/>
+    <mergeCell ref="P265:Q265"/>
+    <mergeCell ref="A262:J262"/>
+    <mergeCell ref="K262:M262"/>
+    <mergeCell ref="N262:O262"/>
+    <mergeCell ref="P262:Q262"/>
+    <mergeCell ref="A263:J263"/>
+    <mergeCell ref="K263:M263"/>
+    <mergeCell ref="N263:O263"/>
+    <mergeCell ref="P263:Q263"/>
+    <mergeCell ref="A260:J260"/>
+    <mergeCell ref="K260:M260"/>
+    <mergeCell ref="N260:O260"/>
+    <mergeCell ref="P260:Q260"/>
+    <mergeCell ref="A261:J261"/>
+    <mergeCell ref="K261:M261"/>
+    <mergeCell ref="N261:O261"/>
+    <mergeCell ref="P261:Q261"/>
+    <mergeCell ref="A258:J258"/>
+    <mergeCell ref="K258:M258"/>
+    <mergeCell ref="N258:O258"/>
+    <mergeCell ref="P258:Q258"/>
+    <mergeCell ref="A259:J259"/>
+    <mergeCell ref="K259:M259"/>
+    <mergeCell ref="N259:O259"/>
+    <mergeCell ref="P259:Q259"/>
+    <mergeCell ref="A256:J256"/>
+    <mergeCell ref="K256:M256"/>
+    <mergeCell ref="N256:O256"/>
+    <mergeCell ref="P256:Q256"/>
+    <mergeCell ref="A257:J257"/>
+    <mergeCell ref="K257:M257"/>
+    <mergeCell ref="N257:O257"/>
+    <mergeCell ref="P257:Q257"/>
+    <mergeCell ref="A254:J254"/>
+    <mergeCell ref="K254:M254"/>
+    <mergeCell ref="N254:O254"/>
+    <mergeCell ref="P254:Q254"/>
+    <mergeCell ref="A255:J255"/>
+    <mergeCell ref="K255:M255"/>
+    <mergeCell ref="N255:O255"/>
+    <mergeCell ref="P255:Q255"/>
+    <mergeCell ref="A252:J252"/>
+    <mergeCell ref="K252:M252"/>
+    <mergeCell ref="N252:O252"/>
+    <mergeCell ref="P252:Q252"/>
+    <mergeCell ref="A253:J253"/>
+    <mergeCell ref="K253:M253"/>
+    <mergeCell ref="N253:O253"/>
+    <mergeCell ref="P253:Q253"/>
+    <mergeCell ref="A250:J250"/>
+    <mergeCell ref="K250:M250"/>
+    <mergeCell ref="N250:O250"/>
+    <mergeCell ref="P250:Q250"/>
+    <mergeCell ref="A251:J251"/>
+    <mergeCell ref="K251:M251"/>
+    <mergeCell ref="N251:O251"/>
+    <mergeCell ref="P251:Q251"/>
+    <mergeCell ref="A248:J248"/>
+    <mergeCell ref="K248:M248"/>
+    <mergeCell ref="N248:O248"/>
+    <mergeCell ref="P248:Q248"/>
+    <mergeCell ref="A249:J249"/>
+    <mergeCell ref="K249:M249"/>
+    <mergeCell ref="N249:O249"/>
+    <mergeCell ref="P249:Q249"/>
+    <mergeCell ref="A246:J246"/>
+    <mergeCell ref="K246:M246"/>
+    <mergeCell ref="N246:O246"/>
+    <mergeCell ref="P246:Q246"/>
+    <mergeCell ref="A247:J247"/>
+    <mergeCell ref="K247:M247"/>
+    <mergeCell ref="N247:O247"/>
+    <mergeCell ref="P247:Q247"/>
+    <mergeCell ref="A244:J244"/>
+    <mergeCell ref="K244:M244"/>
+    <mergeCell ref="N244:O244"/>
+    <mergeCell ref="P244:Q244"/>
+    <mergeCell ref="A245:J245"/>
+    <mergeCell ref="K245:M245"/>
+    <mergeCell ref="N245:O245"/>
+    <mergeCell ref="P245:Q245"/>
+    <mergeCell ref="A242:J242"/>
+    <mergeCell ref="K242:M242"/>
+    <mergeCell ref="N242:O242"/>
+    <mergeCell ref="P242:Q242"/>
+    <mergeCell ref="A243:J243"/>
+    <mergeCell ref="K243:M243"/>
+    <mergeCell ref="N243:O243"/>
+    <mergeCell ref="P243:Q243"/>
+    <mergeCell ref="A240:J240"/>
+    <mergeCell ref="K240:M240"/>
+    <mergeCell ref="N240:O240"/>
+    <mergeCell ref="P240:Q240"/>
+    <mergeCell ref="A241:J241"/>
+    <mergeCell ref="K241:M241"/>
+    <mergeCell ref="N241:O241"/>
+    <mergeCell ref="P241:Q241"/>
+    <mergeCell ref="A238:J238"/>
+    <mergeCell ref="K238:M238"/>
+    <mergeCell ref="N238:O238"/>
+    <mergeCell ref="P238:Q238"/>
+    <mergeCell ref="A239:J239"/>
+    <mergeCell ref="K239:M239"/>
+    <mergeCell ref="N239:O239"/>
+    <mergeCell ref="P239:Q239"/>
+    <mergeCell ref="A236:J236"/>
+    <mergeCell ref="K236:M236"/>
+    <mergeCell ref="N236:O236"/>
+    <mergeCell ref="P236:Q236"/>
+    <mergeCell ref="A237:J237"/>
+    <mergeCell ref="K237:M237"/>
+    <mergeCell ref="N237:O237"/>
+    <mergeCell ref="P237:Q237"/>
+    <mergeCell ref="A234:J234"/>
+    <mergeCell ref="K234:M234"/>
+    <mergeCell ref="N234:O234"/>
+    <mergeCell ref="P234:Q234"/>
+    <mergeCell ref="A235:J235"/>
+    <mergeCell ref="K235:M235"/>
+    <mergeCell ref="N235:O235"/>
+    <mergeCell ref="P235:Q235"/>
+    <mergeCell ref="A232:J232"/>
+    <mergeCell ref="K232:M232"/>
+    <mergeCell ref="N232:O232"/>
+    <mergeCell ref="P232:Q232"/>
+    <mergeCell ref="A233:J233"/>
+    <mergeCell ref="K233:M233"/>
+    <mergeCell ref="N233:O233"/>
+    <mergeCell ref="P233:Q233"/>
+    <mergeCell ref="A230:J230"/>
+    <mergeCell ref="K230:M230"/>
+    <mergeCell ref="N230:O230"/>
+    <mergeCell ref="P230:Q230"/>
+    <mergeCell ref="A231:J231"/>
+    <mergeCell ref="K231:M231"/>
+    <mergeCell ref="N231:O231"/>
+    <mergeCell ref="P231:Q231"/>
+    <mergeCell ref="A228:J228"/>
+    <mergeCell ref="K228:M228"/>
+    <mergeCell ref="N228:O228"/>
+    <mergeCell ref="P228:Q228"/>
+    <mergeCell ref="A229:J229"/>
+    <mergeCell ref="K229:M229"/>
+    <mergeCell ref="N229:O229"/>
+    <mergeCell ref="P229:Q229"/>
+    <mergeCell ref="A226:J226"/>
+    <mergeCell ref="K226:M226"/>
+    <mergeCell ref="N226:O226"/>
+    <mergeCell ref="P226:Q226"/>
+    <mergeCell ref="A227:J227"/>
+    <mergeCell ref="K227:M227"/>
+    <mergeCell ref="N227:O227"/>
+    <mergeCell ref="P227:Q227"/>
+    <mergeCell ref="A224:J224"/>
+    <mergeCell ref="K224:M224"/>
+    <mergeCell ref="N224:O224"/>
+    <mergeCell ref="P224:Q224"/>
+    <mergeCell ref="A225:J225"/>
+    <mergeCell ref="K225:M225"/>
+    <mergeCell ref="N225:O225"/>
+    <mergeCell ref="P225:Q225"/>
+    <mergeCell ref="A222:J222"/>
+    <mergeCell ref="K222:M222"/>
+    <mergeCell ref="N222:O222"/>
+    <mergeCell ref="P222:Q222"/>
+    <mergeCell ref="A223:J223"/>
+    <mergeCell ref="K223:M223"/>
+    <mergeCell ref="N223:O223"/>
+    <mergeCell ref="P223:Q223"/>
+    <mergeCell ref="A220:J220"/>
+    <mergeCell ref="K220:M220"/>
+    <mergeCell ref="N220:O220"/>
+    <mergeCell ref="P220:Q220"/>
+    <mergeCell ref="A221:J221"/>
+    <mergeCell ref="K221:M221"/>
+    <mergeCell ref="N221:O221"/>
+    <mergeCell ref="P221:Q221"/>
+    <mergeCell ref="A218:J218"/>
+    <mergeCell ref="K218:M218"/>
+    <mergeCell ref="N218:O218"/>
+    <mergeCell ref="P218:Q218"/>
+    <mergeCell ref="A219:J219"/>
+    <mergeCell ref="K219:M219"/>
+    <mergeCell ref="N219:O219"/>
+    <mergeCell ref="P219:Q219"/>
+    <mergeCell ref="A216:J216"/>
+    <mergeCell ref="K216:M216"/>
+    <mergeCell ref="N216:O216"/>
+    <mergeCell ref="P216:Q216"/>
+    <mergeCell ref="A217:J217"/>
+    <mergeCell ref="K217:M217"/>
+    <mergeCell ref="N217:O217"/>
+    <mergeCell ref="P217:Q217"/>
+    <mergeCell ref="A214:J214"/>
+    <mergeCell ref="K214:M214"/>
+    <mergeCell ref="N214:O214"/>
+    <mergeCell ref="P214:Q214"/>
+    <mergeCell ref="A215:J215"/>
+    <mergeCell ref="K215:M215"/>
+    <mergeCell ref="N215:O215"/>
+    <mergeCell ref="P215:Q215"/>
+    <mergeCell ref="A212:J212"/>
+    <mergeCell ref="K212:M212"/>
+    <mergeCell ref="N212:O212"/>
+    <mergeCell ref="P212:Q212"/>
+    <mergeCell ref="A213:J213"/>
+    <mergeCell ref="K213:M213"/>
+    <mergeCell ref="N213:O213"/>
+    <mergeCell ref="P213:Q213"/>
+    <mergeCell ref="A210:J210"/>
+    <mergeCell ref="K210:M210"/>
+    <mergeCell ref="N210:O210"/>
+    <mergeCell ref="P210:Q210"/>
+    <mergeCell ref="A211:J211"/>
+    <mergeCell ref="K211:M211"/>
+    <mergeCell ref="N211:O211"/>
+    <mergeCell ref="P211:Q211"/>
+    <mergeCell ref="A208:J208"/>
+    <mergeCell ref="K208:M208"/>
+    <mergeCell ref="N208:O208"/>
+    <mergeCell ref="P208:Q208"/>
+    <mergeCell ref="A209:J209"/>
+    <mergeCell ref="K209:M209"/>
+    <mergeCell ref="N209:O209"/>
+    <mergeCell ref="P209:Q209"/>
+    <mergeCell ref="A206:J206"/>
+    <mergeCell ref="K206:M206"/>
+    <mergeCell ref="N206:O206"/>
+    <mergeCell ref="P206:Q206"/>
+    <mergeCell ref="A207:J207"/>
+    <mergeCell ref="K207:M207"/>
+    <mergeCell ref="N207:O207"/>
+    <mergeCell ref="P207:Q207"/>
+    <mergeCell ref="A204:J204"/>
+    <mergeCell ref="K204:M204"/>
+    <mergeCell ref="N204:O204"/>
+    <mergeCell ref="P204:Q204"/>
+    <mergeCell ref="A205:J205"/>
+    <mergeCell ref="K205:M205"/>
+    <mergeCell ref="N205:O205"/>
+    <mergeCell ref="P205:Q205"/>
+    <mergeCell ref="A202:J202"/>
+    <mergeCell ref="K202:M202"/>
+    <mergeCell ref="N202:O202"/>
+    <mergeCell ref="P202:Q202"/>
+    <mergeCell ref="A203:J203"/>
+    <mergeCell ref="K203:M203"/>
+    <mergeCell ref="N203:O203"/>
+    <mergeCell ref="P203:Q203"/>
+    <mergeCell ref="A200:J200"/>
+    <mergeCell ref="K200:M200"/>
+    <mergeCell ref="N200:O200"/>
+    <mergeCell ref="P200:Q200"/>
+    <mergeCell ref="A201:J201"/>
+    <mergeCell ref="K201:M201"/>
+    <mergeCell ref="N201:O201"/>
+    <mergeCell ref="P201:Q201"/>
+    <mergeCell ref="A198:J198"/>
+    <mergeCell ref="K198:M198"/>
+    <mergeCell ref="N198:O198"/>
+    <mergeCell ref="P198:Q198"/>
+    <mergeCell ref="A199:J199"/>
+    <mergeCell ref="K199:M199"/>
+    <mergeCell ref="N199:O199"/>
+    <mergeCell ref="P199:Q199"/>
+    <mergeCell ref="A196:J196"/>
+    <mergeCell ref="K196:M196"/>
+    <mergeCell ref="N196:O196"/>
+    <mergeCell ref="P196:Q196"/>
+    <mergeCell ref="A197:J197"/>
+    <mergeCell ref="K197:M197"/>
+    <mergeCell ref="N197:O197"/>
+    <mergeCell ref="P197:Q197"/>
+    <mergeCell ref="A194:J194"/>
+    <mergeCell ref="K194:M194"/>
+    <mergeCell ref="N194:O194"/>
+    <mergeCell ref="P194:Q194"/>
+    <mergeCell ref="A195:J195"/>
+    <mergeCell ref="K195:M195"/>
+    <mergeCell ref="N195:O195"/>
+    <mergeCell ref="P195:Q195"/>
+    <mergeCell ref="A192:J192"/>
+    <mergeCell ref="K192:M192"/>
+    <mergeCell ref="N192:O192"/>
+    <mergeCell ref="P192:Q192"/>
+    <mergeCell ref="A193:J193"/>
+    <mergeCell ref="K193:M193"/>
+    <mergeCell ref="N193:O193"/>
+    <mergeCell ref="P193:Q193"/>
+    <mergeCell ref="A190:J190"/>
+    <mergeCell ref="K190:M190"/>
+    <mergeCell ref="N190:O190"/>
+    <mergeCell ref="P190:Q190"/>
+    <mergeCell ref="A191:J191"/>
+    <mergeCell ref="K191:M191"/>
+    <mergeCell ref="N191:O191"/>
+    <mergeCell ref="P191:Q191"/>
+    <mergeCell ref="A188:J188"/>
+    <mergeCell ref="K188:M188"/>
+    <mergeCell ref="N188:O188"/>
+    <mergeCell ref="P188:Q188"/>
+    <mergeCell ref="A189:J189"/>
+    <mergeCell ref="K189:M189"/>
+    <mergeCell ref="N189:O189"/>
+    <mergeCell ref="P189:Q189"/>
+    <mergeCell ref="A186:J186"/>
+    <mergeCell ref="K186:M186"/>
+    <mergeCell ref="N186:O186"/>
+    <mergeCell ref="P186:Q186"/>
+    <mergeCell ref="A187:J187"/>
+    <mergeCell ref="K187:M187"/>
+    <mergeCell ref="N187:O187"/>
+    <mergeCell ref="P187:Q187"/>
+    <mergeCell ref="A184:J184"/>
+    <mergeCell ref="K184:M184"/>
+    <mergeCell ref="N184:O184"/>
+    <mergeCell ref="P184:Q184"/>
+    <mergeCell ref="A185:J185"/>
+    <mergeCell ref="K185:M185"/>
+    <mergeCell ref="N185:O185"/>
+    <mergeCell ref="P185:Q185"/>
+    <mergeCell ref="A182:J182"/>
+    <mergeCell ref="K182:M182"/>
+    <mergeCell ref="N182:O182"/>
+    <mergeCell ref="P182:Q182"/>
+    <mergeCell ref="A183:J183"/>
+    <mergeCell ref="K183:M183"/>
+    <mergeCell ref="N183:O183"/>
+    <mergeCell ref="P183:Q183"/>
+    <mergeCell ref="A180:J180"/>
+    <mergeCell ref="K180:M180"/>
+    <mergeCell ref="N180:O180"/>
+    <mergeCell ref="P180:Q180"/>
+    <mergeCell ref="A181:J181"/>
+    <mergeCell ref="K181:M181"/>
+    <mergeCell ref="N181:O181"/>
+    <mergeCell ref="P181:Q181"/>
+    <mergeCell ref="A178:J178"/>
+    <mergeCell ref="K178:M178"/>
+    <mergeCell ref="N178:O178"/>
+    <mergeCell ref="P178:Q178"/>
+    <mergeCell ref="A179:J179"/>
+    <mergeCell ref="K179:M179"/>
+    <mergeCell ref="N179:O179"/>
+    <mergeCell ref="P179:Q179"/>
+    <mergeCell ref="A176:J176"/>
+    <mergeCell ref="K176:M176"/>
+    <mergeCell ref="N176:O176"/>
+    <mergeCell ref="P176:Q176"/>
+    <mergeCell ref="A177:J177"/>
+    <mergeCell ref="K177:M177"/>
+    <mergeCell ref="N177:O177"/>
+    <mergeCell ref="P177:Q177"/>
+    <mergeCell ref="A174:J174"/>
+    <mergeCell ref="K174:M174"/>
+    <mergeCell ref="N174:O174"/>
+    <mergeCell ref="P174:Q174"/>
+    <mergeCell ref="A175:J175"/>
+    <mergeCell ref="K175:M175"/>
+    <mergeCell ref="N175:O175"/>
+    <mergeCell ref="P175:Q175"/>
+    <mergeCell ref="A172:J172"/>
+    <mergeCell ref="K172:M172"/>
+    <mergeCell ref="N172:O172"/>
+    <mergeCell ref="P172:Q172"/>
+    <mergeCell ref="A173:J173"/>
+    <mergeCell ref="K173:M173"/>
+    <mergeCell ref="N173:O173"/>
+    <mergeCell ref="P173:Q173"/>
+    <mergeCell ref="A170:J170"/>
+    <mergeCell ref="K170:M170"/>
+    <mergeCell ref="N170:O170"/>
+    <mergeCell ref="P170:Q170"/>
+    <mergeCell ref="A171:J171"/>
+    <mergeCell ref="K171:M171"/>
+    <mergeCell ref="N171:O171"/>
+    <mergeCell ref="P171:Q171"/>
+    <mergeCell ref="A168:J168"/>
+    <mergeCell ref="K168:M168"/>
+    <mergeCell ref="N168:O168"/>
+    <mergeCell ref="P168:Q168"/>
+    <mergeCell ref="A169:J169"/>
+    <mergeCell ref="K169:M169"/>
+    <mergeCell ref="N169:O169"/>
+    <mergeCell ref="P169:Q169"/>
+    <mergeCell ref="A166:J166"/>
+    <mergeCell ref="K166:M166"/>
+    <mergeCell ref="N166:O166"/>
+    <mergeCell ref="P166:Q166"/>
+    <mergeCell ref="A167:J167"/>
+    <mergeCell ref="K167:M167"/>
+    <mergeCell ref="N167:O167"/>
+    <mergeCell ref="P167:Q167"/>
+    <mergeCell ref="A164:J164"/>
+    <mergeCell ref="K164:M164"/>
+    <mergeCell ref="N164:O164"/>
+    <mergeCell ref="P164:Q164"/>
+    <mergeCell ref="A165:J165"/>
+    <mergeCell ref="K165:M165"/>
+    <mergeCell ref="N165:O165"/>
+    <mergeCell ref="P165:Q165"/>
+    <mergeCell ref="A162:J162"/>
+    <mergeCell ref="K162:M162"/>
+    <mergeCell ref="N162:O162"/>
+    <mergeCell ref="P162:Q162"/>
+    <mergeCell ref="A163:J163"/>
+    <mergeCell ref="K163:M163"/>
+    <mergeCell ref="N163:O163"/>
+    <mergeCell ref="P163:Q163"/>
+    <mergeCell ref="A160:J160"/>
+    <mergeCell ref="K160:M160"/>
+    <mergeCell ref="N160:O160"/>
+    <mergeCell ref="P160:Q160"/>
+    <mergeCell ref="A161:J161"/>
+    <mergeCell ref="K161:M161"/>
+    <mergeCell ref="N161:O161"/>
+    <mergeCell ref="P161:Q161"/>
+    <mergeCell ref="A158:J158"/>
+    <mergeCell ref="K158:M158"/>
+    <mergeCell ref="N158:O158"/>
+    <mergeCell ref="P158:Q158"/>
+    <mergeCell ref="A159:J159"/>
+    <mergeCell ref="K159:M159"/>
+    <mergeCell ref="N159:O159"/>
+    <mergeCell ref="P159:Q159"/>
+    <mergeCell ref="A156:J156"/>
+    <mergeCell ref="K156:M156"/>
+    <mergeCell ref="N156:O156"/>
+    <mergeCell ref="P156:Q156"/>
+    <mergeCell ref="A157:J157"/>
+    <mergeCell ref="K157:M157"/>
+    <mergeCell ref="N157:O157"/>
+    <mergeCell ref="P157:Q157"/>
+    <mergeCell ref="A154:J154"/>
+    <mergeCell ref="K154:M154"/>
+    <mergeCell ref="N154:O154"/>
+    <mergeCell ref="P154:Q154"/>
+    <mergeCell ref="A155:J155"/>
+    <mergeCell ref="K155:M155"/>
+    <mergeCell ref="N155:O155"/>
+    <mergeCell ref="P155:Q155"/>
+    <mergeCell ref="A152:J152"/>
+    <mergeCell ref="K152:M152"/>
+    <mergeCell ref="N152:O152"/>
+    <mergeCell ref="P152:Q152"/>
+    <mergeCell ref="A153:J153"/>
+    <mergeCell ref="K153:M153"/>
+    <mergeCell ref="N153:O153"/>
+    <mergeCell ref="P153:Q153"/>
+    <mergeCell ref="A150:J150"/>
+    <mergeCell ref="K150:M150"/>
+    <mergeCell ref="N150:O150"/>
+    <mergeCell ref="P150:Q150"/>
+    <mergeCell ref="A151:J151"/>
+    <mergeCell ref="K151:M151"/>
+    <mergeCell ref="N151:O151"/>
+    <mergeCell ref="P151:Q151"/>
+    <mergeCell ref="A148:J148"/>
+    <mergeCell ref="K148:M148"/>
+    <mergeCell ref="N148:O148"/>
+    <mergeCell ref="P148:Q148"/>
+    <mergeCell ref="A149:J149"/>
+    <mergeCell ref="K149:M149"/>
+    <mergeCell ref="N149:O149"/>
+    <mergeCell ref="P149:Q149"/>
+    <mergeCell ref="A146:J146"/>
+    <mergeCell ref="K146:M146"/>
+    <mergeCell ref="N146:O146"/>
+    <mergeCell ref="P146:Q146"/>
+    <mergeCell ref="A147:J147"/>
+    <mergeCell ref="K147:M147"/>
+    <mergeCell ref="N147:O147"/>
+    <mergeCell ref="P147:Q147"/>
+    <mergeCell ref="A144:J144"/>
+    <mergeCell ref="K144:M144"/>
+    <mergeCell ref="N144:O144"/>
+    <mergeCell ref="P144:Q144"/>
+    <mergeCell ref="A145:J145"/>
+    <mergeCell ref="K145:M145"/>
+    <mergeCell ref="N145:O145"/>
+    <mergeCell ref="P145:Q145"/>
+    <mergeCell ref="A142:J142"/>
+    <mergeCell ref="K142:M142"/>
+    <mergeCell ref="N142:O142"/>
+    <mergeCell ref="P142:Q142"/>
+    <mergeCell ref="A143:J143"/>
+    <mergeCell ref="K143:M143"/>
+    <mergeCell ref="N143:O143"/>
+    <mergeCell ref="P143:Q143"/>
+    <mergeCell ref="A140:J140"/>
+    <mergeCell ref="K140:M140"/>
+    <mergeCell ref="N140:O140"/>
+    <mergeCell ref="P140:Q140"/>
+    <mergeCell ref="A141:J141"/>
+    <mergeCell ref="K141:M141"/>
+    <mergeCell ref="N141:O141"/>
+    <mergeCell ref="P141:Q141"/>
+    <mergeCell ref="A138:J138"/>
+    <mergeCell ref="K138:M138"/>
+    <mergeCell ref="N138:O138"/>
+    <mergeCell ref="P138:Q138"/>
+    <mergeCell ref="A139:J139"/>
+    <mergeCell ref="K139:M139"/>
+    <mergeCell ref="N139:O139"/>
+    <mergeCell ref="P139:Q139"/>
+    <mergeCell ref="A136:J136"/>
+    <mergeCell ref="K136:M136"/>
+    <mergeCell ref="N136:O136"/>
+    <mergeCell ref="P136:Q136"/>
+    <mergeCell ref="A137:J137"/>
+    <mergeCell ref="K137:M137"/>
+    <mergeCell ref="N137:O137"/>
+    <mergeCell ref="P137:Q137"/>
+    <mergeCell ref="A134:J134"/>
+    <mergeCell ref="K134:M134"/>
+    <mergeCell ref="N134:O134"/>
+    <mergeCell ref="P134:Q134"/>
+    <mergeCell ref="A135:J135"/>
+    <mergeCell ref="K135:M135"/>
+    <mergeCell ref="N135:O135"/>
+    <mergeCell ref="P135:Q135"/>
+    <mergeCell ref="A132:J132"/>
+    <mergeCell ref="K132:M132"/>
+    <mergeCell ref="N132:O132"/>
+    <mergeCell ref="P132:Q132"/>
+    <mergeCell ref="A133:J133"/>
+    <mergeCell ref="K133:M133"/>
+    <mergeCell ref="N133:O133"/>
+    <mergeCell ref="P133:Q133"/>
+    <mergeCell ref="A130:J130"/>
+    <mergeCell ref="K130:M130"/>
+    <mergeCell ref="N130:O130"/>
+    <mergeCell ref="P130:Q130"/>
+    <mergeCell ref="A131:J131"/>
+    <mergeCell ref="K131:M131"/>
+    <mergeCell ref="N131:O131"/>
+    <mergeCell ref="P131:Q131"/>
+    <mergeCell ref="A128:J128"/>
+    <mergeCell ref="K128:M128"/>
+    <mergeCell ref="N128:O128"/>
+    <mergeCell ref="P128:Q128"/>
+    <mergeCell ref="A129:J129"/>
+    <mergeCell ref="K129:M129"/>
+    <mergeCell ref="N129:O129"/>
+    <mergeCell ref="P129:Q129"/>
+    <mergeCell ref="A126:J126"/>
+    <mergeCell ref="K126:M126"/>
+    <mergeCell ref="N126:O126"/>
+    <mergeCell ref="P126:Q126"/>
+    <mergeCell ref="A127:J127"/>
+    <mergeCell ref="K127:M127"/>
+    <mergeCell ref="N127:O127"/>
+    <mergeCell ref="P127:Q127"/>
+    <mergeCell ref="A124:J124"/>
+    <mergeCell ref="K124:M124"/>
+    <mergeCell ref="N124:O124"/>
+    <mergeCell ref="P124:Q124"/>
+    <mergeCell ref="A125:J125"/>
+    <mergeCell ref="K125:M125"/>
+    <mergeCell ref="N125:O125"/>
+    <mergeCell ref="P125:Q125"/>
+    <mergeCell ref="A122:J122"/>
+    <mergeCell ref="K122:M122"/>
+    <mergeCell ref="N122:O122"/>
+    <mergeCell ref="P122:Q122"/>
+    <mergeCell ref="A123:J123"/>
+    <mergeCell ref="K123:M123"/>
+    <mergeCell ref="N123:O123"/>
+    <mergeCell ref="P123:Q123"/>
+    <mergeCell ref="A120:J120"/>
+    <mergeCell ref="K120:M120"/>
+    <mergeCell ref="N120:O120"/>
+    <mergeCell ref="P120:Q120"/>
+    <mergeCell ref="A121:J121"/>
+    <mergeCell ref="K121:M121"/>
+    <mergeCell ref="N121:O121"/>
+    <mergeCell ref="P121:Q121"/>
+    <mergeCell ref="A118:J118"/>
+    <mergeCell ref="K118:M118"/>
+    <mergeCell ref="N118:O118"/>
+    <mergeCell ref="P118:Q118"/>
+    <mergeCell ref="A119:J119"/>
+    <mergeCell ref="K119:M119"/>
+    <mergeCell ref="N119:O119"/>
+    <mergeCell ref="P119:Q119"/>
+    <mergeCell ref="A116:J116"/>
+    <mergeCell ref="K116:M116"/>
+    <mergeCell ref="N116:O116"/>
+    <mergeCell ref="P116:Q116"/>
+    <mergeCell ref="A117:J117"/>
+    <mergeCell ref="K117:M117"/>
+    <mergeCell ref="N117:O117"/>
+    <mergeCell ref="P117:Q117"/>
+    <mergeCell ref="A114:J114"/>
+    <mergeCell ref="K114:M114"/>
+    <mergeCell ref="N114:O114"/>
+    <mergeCell ref="P114:Q114"/>
+    <mergeCell ref="A115:J115"/>
+    <mergeCell ref="K115:M115"/>
+    <mergeCell ref="N115:O115"/>
+    <mergeCell ref="P115:Q115"/>
+    <mergeCell ref="A112:J112"/>
+    <mergeCell ref="K112:M112"/>
+    <mergeCell ref="N112:O112"/>
+    <mergeCell ref="P112:Q112"/>
+    <mergeCell ref="A113:J113"/>
+    <mergeCell ref="K113:M113"/>
+    <mergeCell ref="N113:O113"/>
+    <mergeCell ref="P113:Q113"/>
+    <mergeCell ref="A110:J110"/>
+    <mergeCell ref="K110:M110"/>
+    <mergeCell ref="N110:O110"/>
+    <mergeCell ref="P110:Q110"/>
+    <mergeCell ref="A111:J111"/>
+    <mergeCell ref="K111:M111"/>
+    <mergeCell ref="N111:O111"/>
+    <mergeCell ref="P111:Q111"/>
+    <mergeCell ref="A108:J108"/>
+    <mergeCell ref="K108:M108"/>
+    <mergeCell ref="N108:O108"/>
+    <mergeCell ref="P108:Q108"/>
+    <mergeCell ref="A109:J109"/>
+    <mergeCell ref="K109:M109"/>
+    <mergeCell ref="N109:O109"/>
+    <mergeCell ref="P109:Q109"/>
+    <mergeCell ref="A106:J106"/>
+    <mergeCell ref="K106:M106"/>
+    <mergeCell ref="N106:O106"/>
+    <mergeCell ref="P106:Q106"/>
+    <mergeCell ref="A107:J107"/>
+    <mergeCell ref="K107:M107"/>
+    <mergeCell ref="N107:O107"/>
+    <mergeCell ref="P107:Q107"/>
+    <mergeCell ref="A104:J104"/>
+    <mergeCell ref="K104:M104"/>
+    <mergeCell ref="N104:O104"/>
+    <mergeCell ref="P104:Q104"/>
+    <mergeCell ref="A105:J105"/>
+    <mergeCell ref="K105:M105"/>
+    <mergeCell ref="N105:O105"/>
+    <mergeCell ref="P105:Q105"/>
+    <mergeCell ref="A102:J102"/>
+    <mergeCell ref="K102:M102"/>
+    <mergeCell ref="N102:O102"/>
+    <mergeCell ref="P102:Q102"/>
+    <mergeCell ref="A103:J103"/>
+    <mergeCell ref="K103:M103"/>
+    <mergeCell ref="N103:O103"/>
+    <mergeCell ref="P103:Q103"/>
+    <mergeCell ref="A100:J100"/>
+    <mergeCell ref="K100:M100"/>
+    <mergeCell ref="N100:O100"/>
+    <mergeCell ref="P100:Q100"/>
+    <mergeCell ref="A101:J101"/>
+    <mergeCell ref="K101:M101"/>
+    <mergeCell ref="N101:O101"/>
+    <mergeCell ref="P101:Q101"/>
+    <mergeCell ref="A98:J98"/>
+    <mergeCell ref="K98:M98"/>
+    <mergeCell ref="N98:O98"/>
+    <mergeCell ref="P98:Q98"/>
+    <mergeCell ref="A99:J99"/>
+    <mergeCell ref="K99:M99"/>
+    <mergeCell ref="N99:O99"/>
+    <mergeCell ref="P99:Q99"/>
+    <mergeCell ref="A96:J96"/>
+    <mergeCell ref="K96:M96"/>
+    <mergeCell ref="N96:O96"/>
+    <mergeCell ref="P96:Q96"/>
+    <mergeCell ref="A97:J97"/>
+    <mergeCell ref="K97:M97"/>
+    <mergeCell ref="N97:O97"/>
+    <mergeCell ref="P97:Q97"/>
+    <mergeCell ref="A94:J94"/>
+    <mergeCell ref="K94:M94"/>
+    <mergeCell ref="N94:O94"/>
+    <mergeCell ref="P94:Q94"/>
+    <mergeCell ref="A95:J95"/>
+    <mergeCell ref="K95:M95"/>
+    <mergeCell ref="N95:O95"/>
+    <mergeCell ref="P95:Q95"/>
+    <mergeCell ref="A92:J92"/>
+    <mergeCell ref="K92:M92"/>
+    <mergeCell ref="N92:O92"/>
+    <mergeCell ref="P92:Q92"/>
+    <mergeCell ref="A93:J93"/>
+    <mergeCell ref="K93:M93"/>
+    <mergeCell ref="N93:O93"/>
+    <mergeCell ref="P93:Q93"/>
+    <mergeCell ref="A90:J90"/>
+    <mergeCell ref="K90:M90"/>
+    <mergeCell ref="N90:O90"/>
+    <mergeCell ref="P90:Q90"/>
+    <mergeCell ref="A91:J91"/>
+    <mergeCell ref="K91:M91"/>
+    <mergeCell ref="N91:O91"/>
+    <mergeCell ref="P91:Q91"/>
+    <mergeCell ref="A88:J88"/>
+    <mergeCell ref="K88:M88"/>
+    <mergeCell ref="N88:O88"/>
+    <mergeCell ref="P88:Q88"/>
+    <mergeCell ref="A89:J89"/>
+    <mergeCell ref="K89:M89"/>
+    <mergeCell ref="N89:O89"/>
+    <mergeCell ref="P89:Q89"/>
+    <mergeCell ref="A86:J86"/>
+    <mergeCell ref="K86:M86"/>
+    <mergeCell ref="N86:O86"/>
+    <mergeCell ref="P86:Q86"/>
+    <mergeCell ref="A87:J87"/>
+    <mergeCell ref="K87:M87"/>
+    <mergeCell ref="N87:O87"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="A84:J84"/>
+    <mergeCell ref="K84:M84"/>
+    <mergeCell ref="N84:O84"/>
+    <mergeCell ref="P84:Q84"/>
+    <mergeCell ref="A85:J85"/>
+    <mergeCell ref="K85:M85"/>
+    <mergeCell ref="N85:O85"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="A82:J82"/>
+    <mergeCell ref="K82:M82"/>
+    <mergeCell ref="N82:O82"/>
+    <mergeCell ref="P82:Q82"/>
+    <mergeCell ref="A83:J83"/>
+    <mergeCell ref="K83:M83"/>
+    <mergeCell ref="N83:O83"/>
+    <mergeCell ref="P83:Q83"/>
+    <mergeCell ref="A80:J80"/>
+    <mergeCell ref="K80:M80"/>
+    <mergeCell ref="N80:O80"/>
+    <mergeCell ref="P80:Q80"/>
+    <mergeCell ref="A81:J81"/>
+    <mergeCell ref="K81:M81"/>
+    <mergeCell ref="N81:O81"/>
+    <mergeCell ref="P81:Q81"/>
+    <mergeCell ref="A78:J78"/>
+    <mergeCell ref="K78:M78"/>
+    <mergeCell ref="N78:O78"/>
+    <mergeCell ref="P78:Q78"/>
+    <mergeCell ref="A79:J79"/>
+    <mergeCell ref="K79:M79"/>
+    <mergeCell ref="N79:O79"/>
+    <mergeCell ref="P79:Q79"/>
+    <mergeCell ref="A76:J76"/>
+    <mergeCell ref="K76:M76"/>
+    <mergeCell ref="N76:O76"/>
+    <mergeCell ref="P76:Q76"/>
+    <mergeCell ref="A77:J77"/>
+    <mergeCell ref="K77:M77"/>
+    <mergeCell ref="N77:O77"/>
+    <mergeCell ref="P77:Q77"/>
+    <mergeCell ref="A74:J74"/>
+    <mergeCell ref="K74:M74"/>
+    <mergeCell ref="N74:O74"/>
+    <mergeCell ref="P74:Q74"/>
+    <mergeCell ref="A75:J75"/>
+    <mergeCell ref="K75:M75"/>
+    <mergeCell ref="N75:O75"/>
+    <mergeCell ref="P75:Q75"/>
+    <mergeCell ref="A72:J72"/>
+    <mergeCell ref="K72:M72"/>
+    <mergeCell ref="N72:O72"/>
+    <mergeCell ref="P72:Q72"/>
+    <mergeCell ref="A73:J73"/>
+    <mergeCell ref="K73:M73"/>
+    <mergeCell ref="N73:O73"/>
+    <mergeCell ref="P73:Q73"/>
+    <mergeCell ref="A70:J70"/>
+    <mergeCell ref="K70:M70"/>
+    <mergeCell ref="N70:O70"/>
+    <mergeCell ref="P70:Q70"/>
+    <mergeCell ref="A71:J71"/>
+    <mergeCell ref="K71:M71"/>
+    <mergeCell ref="N71:O71"/>
+    <mergeCell ref="P71:Q71"/>
+    <mergeCell ref="A68:J68"/>
+    <mergeCell ref="K68:M68"/>
+    <mergeCell ref="N68:O68"/>
+    <mergeCell ref="P68:Q68"/>
+    <mergeCell ref="A69:J69"/>
+    <mergeCell ref="K69:M69"/>
+    <mergeCell ref="N69:O69"/>
+    <mergeCell ref="P69:Q69"/>
+    <mergeCell ref="A66:J66"/>
+    <mergeCell ref="K66:M66"/>
+    <mergeCell ref="N66:O66"/>
+    <mergeCell ref="P66:Q66"/>
+    <mergeCell ref="A67:J67"/>
+    <mergeCell ref="K67:M67"/>
+    <mergeCell ref="N67:O67"/>
+    <mergeCell ref="P67:Q67"/>
+    <mergeCell ref="A64:J64"/>
+    <mergeCell ref="K64:M64"/>
+    <mergeCell ref="N64:O64"/>
+    <mergeCell ref="P64:Q64"/>
+    <mergeCell ref="A65:J65"/>
+    <mergeCell ref="K65:M65"/>
+    <mergeCell ref="N65:O65"/>
+    <mergeCell ref="P65:Q65"/>
+    <mergeCell ref="A62:J62"/>
+    <mergeCell ref="K62:M62"/>
+    <mergeCell ref="N62:O62"/>
+    <mergeCell ref="P62:Q62"/>
+    <mergeCell ref="A63:J63"/>
+    <mergeCell ref="K63:M63"/>
+    <mergeCell ref="N63:O63"/>
+    <mergeCell ref="P63:Q63"/>
+    <mergeCell ref="A60:J60"/>
+    <mergeCell ref="K60:M60"/>
+    <mergeCell ref="N60:O60"/>
+    <mergeCell ref="P60:Q60"/>
+    <mergeCell ref="A61:J61"/>
+    <mergeCell ref="K61:M61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="P61:Q61"/>
+    <mergeCell ref="A58:J58"/>
+    <mergeCell ref="K58:M58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="P58:Q58"/>
+    <mergeCell ref="A59:J59"/>
+    <mergeCell ref="K59:M59"/>
+    <mergeCell ref="N59:O59"/>
+    <mergeCell ref="P59:Q59"/>
+    <mergeCell ref="A56:J56"/>
+    <mergeCell ref="K56:M56"/>
+    <mergeCell ref="N56:O56"/>
+    <mergeCell ref="P56:Q56"/>
+    <mergeCell ref="A57:J57"/>
+    <mergeCell ref="K57:M57"/>
+    <mergeCell ref="N57:O57"/>
+    <mergeCell ref="P57:Q57"/>
+    <mergeCell ref="A54:J54"/>
+    <mergeCell ref="K54:M54"/>
+    <mergeCell ref="N54:O54"/>
+    <mergeCell ref="P54:Q54"/>
+    <mergeCell ref="A55:J55"/>
+    <mergeCell ref="K55:M55"/>
+    <mergeCell ref="N55:O55"/>
+    <mergeCell ref="P55:Q55"/>
+    <mergeCell ref="A52:J52"/>
+    <mergeCell ref="K52:M52"/>
+    <mergeCell ref="N52:O52"/>
+    <mergeCell ref="P52:Q52"/>
+    <mergeCell ref="A53:J53"/>
+    <mergeCell ref="K53:M53"/>
+    <mergeCell ref="N53:O53"/>
+    <mergeCell ref="P53:Q53"/>
+    <mergeCell ref="A50:J50"/>
+    <mergeCell ref="K50:M50"/>
+    <mergeCell ref="N50:O50"/>
+    <mergeCell ref="P50:Q50"/>
+    <mergeCell ref="A51:J51"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="N51:O51"/>
+    <mergeCell ref="P51:Q51"/>
+    <mergeCell ref="A48:J48"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="P48:Q48"/>
+    <mergeCell ref="A49:J49"/>
+    <mergeCell ref="K49:M49"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="P49:Q49"/>
+    <mergeCell ref="A46:J46"/>
+    <mergeCell ref="K46:M46"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="P46:Q46"/>
+    <mergeCell ref="A47:J47"/>
+    <mergeCell ref="K47:M47"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="A44:J44"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="A45:J45"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="P45:Q45"/>
+    <mergeCell ref="A42:J42"/>
+    <mergeCell ref="K42:M42"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="P42:Q42"/>
+    <mergeCell ref="A43:J43"/>
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="A40:J40"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="P40:Q40"/>
+    <mergeCell ref="A41:J41"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="P41:Q41"/>
+    <mergeCell ref="A38:J38"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="A39:J39"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="A36:J36"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="P36:Q36"/>
+    <mergeCell ref="A37:J37"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="A34:J34"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="A35:J35"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="A32:J32"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="A33:J33"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="A25:J25"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="A21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
     <mergeCell ref="A18:J18"/>
     <mergeCell ref="K18:M18"/>
     <mergeCell ref="N18:O18"/>
@@ -8604,1566 +10153,28 @@
     <mergeCell ref="K15:M15"/>
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="A25:J25"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="A22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="A20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="A21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="K31:M31"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="A26:J26"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="A36:J36"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="P36:Q36"/>
-    <mergeCell ref="A37:J37"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="P37:Q37"/>
-    <mergeCell ref="A34:J34"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="P34:Q34"/>
-    <mergeCell ref="A35:J35"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="P35:Q35"/>
-    <mergeCell ref="A32:J32"/>
-    <mergeCell ref="K32:M32"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="P32:Q32"/>
-    <mergeCell ref="A33:J33"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="P33:Q33"/>
-    <mergeCell ref="A42:J42"/>
-    <mergeCell ref="K42:M42"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="P42:Q42"/>
-    <mergeCell ref="A43:J43"/>
-    <mergeCell ref="K43:M43"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="P43:Q43"/>
-    <mergeCell ref="A40:J40"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="P40:Q40"/>
-    <mergeCell ref="A41:J41"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="P41:Q41"/>
-    <mergeCell ref="A38:J38"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="A39:J39"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="A48:J48"/>
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="N48:O48"/>
-    <mergeCell ref="P48:Q48"/>
-    <mergeCell ref="A49:J49"/>
-    <mergeCell ref="K49:M49"/>
-    <mergeCell ref="N49:O49"/>
-    <mergeCell ref="P49:Q49"/>
-    <mergeCell ref="A46:J46"/>
-    <mergeCell ref="K46:M46"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="P46:Q46"/>
-    <mergeCell ref="A47:J47"/>
-    <mergeCell ref="K47:M47"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="P47:Q47"/>
-    <mergeCell ref="A44:J44"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="P44:Q44"/>
-    <mergeCell ref="A45:J45"/>
-    <mergeCell ref="K45:M45"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="P45:Q45"/>
-    <mergeCell ref="A54:J54"/>
-    <mergeCell ref="K54:M54"/>
-    <mergeCell ref="N54:O54"/>
-    <mergeCell ref="P54:Q54"/>
-    <mergeCell ref="A55:J55"/>
-    <mergeCell ref="K55:M55"/>
-    <mergeCell ref="N55:O55"/>
-    <mergeCell ref="P55:Q55"/>
-    <mergeCell ref="A52:J52"/>
-    <mergeCell ref="K52:M52"/>
-    <mergeCell ref="N52:O52"/>
-    <mergeCell ref="P52:Q52"/>
-    <mergeCell ref="A53:J53"/>
-    <mergeCell ref="K53:M53"/>
-    <mergeCell ref="N53:O53"/>
-    <mergeCell ref="P53:Q53"/>
-    <mergeCell ref="A50:J50"/>
-    <mergeCell ref="K50:M50"/>
-    <mergeCell ref="N50:O50"/>
-    <mergeCell ref="P50:Q50"/>
-    <mergeCell ref="A51:J51"/>
-    <mergeCell ref="K51:M51"/>
-    <mergeCell ref="N51:O51"/>
-    <mergeCell ref="P51:Q51"/>
-    <mergeCell ref="A60:J60"/>
-    <mergeCell ref="K60:M60"/>
-    <mergeCell ref="N60:O60"/>
-    <mergeCell ref="P60:Q60"/>
-    <mergeCell ref="A61:J61"/>
-    <mergeCell ref="K61:M61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="P61:Q61"/>
-    <mergeCell ref="A58:J58"/>
-    <mergeCell ref="K58:M58"/>
-    <mergeCell ref="N58:O58"/>
-    <mergeCell ref="P58:Q58"/>
-    <mergeCell ref="A59:J59"/>
-    <mergeCell ref="K59:M59"/>
-    <mergeCell ref="N59:O59"/>
-    <mergeCell ref="P59:Q59"/>
-    <mergeCell ref="A56:J56"/>
-    <mergeCell ref="K56:M56"/>
-    <mergeCell ref="N56:O56"/>
-    <mergeCell ref="P56:Q56"/>
-    <mergeCell ref="A57:J57"/>
-    <mergeCell ref="K57:M57"/>
-    <mergeCell ref="N57:O57"/>
-    <mergeCell ref="P57:Q57"/>
-    <mergeCell ref="A66:J66"/>
-    <mergeCell ref="K66:M66"/>
-    <mergeCell ref="N66:O66"/>
-    <mergeCell ref="P66:Q66"/>
-    <mergeCell ref="A67:J67"/>
-    <mergeCell ref="K67:M67"/>
-    <mergeCell ref="N67:O67"/>
-    <mergeCell ref="P67:Q67"/>
-    <mergeCell ref="A64:J64"/>
-    <mergeCell ref="K64:M64"/>
-    <mergeCell ref="N64:O64"/>
-    <mergeCell ref="P64:Q64"/>
-    <mergeCell ref="A65:J65"/>
-    <mergeCell ref="K65:M65"/>
-    <mergeCell ref="N65:O65"/>
-    <mergeCell ref="P65:Q65"/>
-    <mergeCell ref="A62:J62"/>
-    <mergeCell ref="K62:M62"/>
-    <mergeCell ref="N62:O62"/>
-    <mergeCell ref="P62:Q62"/>
-    <mergeCell ref="A63:J63"/>
-    <mergeCell ref="K63:M63"/>
-    <mergeCell ref="N63:O63"/>
-    <mergeCell ref="P63:Q63"/>
-    <mergeCell ref="A72:J72"/>
-    <mergeCell ref="K72:M72"/>
-    <mergeCell ref="N72:O72"/>
-    <mergeCell ref="P72:Q72"/>
-    <mergeCell ref="A73:J73"/>
-    <mergeCell ref="K73:M73"/>
-    <mergeCell ref="N73:O73"/>
-    <mergeCell ref="P73:Q73"/>
-    <mergeCell ref="A70:J70"/>
-    <mergeCell ref="K70:M70"/>
-    <mergeCell ref="N70:O70"/>
-    <mergeCell ref="P70:Q70"/>
-    <mergeCell ref="A71:J71"/>
-    <mergeCell ref="K71:M71"/>
-    <mergeCell ref="N71:O71"/>
-    <mergeCell ref="P71:Q71"/>
-    <mergeCell ref="A68:J68"/>
-    <mergeCell ref="K68:M68"/>
-    <mergeCell ref="N68:O68"/>
-    <mergeCell ref="P68:Q68"/>
-    <mergeCell ref="A69:J69"/>
-    <mergeCell ref="K69:M69"/>
-    <mergeCell ref="N69:O69"/>
-    <mergeCell ref="P69:Q69"/>
-    <mergeCell ref="A78:J78"/>
-    <mergeCell ref="K78:M78"/>
-    <mergeCell ref="N78:O78"/>
-    <mergeCell ref="P78:Q78"/>
-    <mergeCell ref="A79:J79"/>
-    <mergeCell ref="K79:M79"/>
-    <mergeCell ref="N79:O79"/>
-    <mergeCell ref="P79:Q79"/>
-    <mergeCell ref="A76:J76"/>
-    <mergeCell ref="K76:M76"/>
-    <mergeCell ref="N76:O76"/>
-    <mergeCell ref="P76:Q76"/>
-    <mergeCell ref="A77:J77"/>
-    <mergeCell ref="K77:M77"/>
-    <mergeCell ref="N77:O77"/>
-    <mergeCell ref="P77:Q77"/>
-    <mergeCell ref="A74:J74"/>
-    <mergeCell ref="K74:M74"/>
-    <mergeCell ref="N74:O74"/>
-    <mergeCell ref="P74:Q74"/>
-    <mergeCell ref="A75:J75"/>
-    <mergeCell ref="K75:M75"/>
-    <mergeCell ref="N75:O75"/>
-    <mergeCell ref="P75:Q75"/>
-    <mergeCell ref="A84:J84"/>
-    <mergeCell ref="K84:M84"/>
-    <mergeCell ref="N84:O84"/>
-    <mergeCell ref="P84:Q84"/>
-    <mergeCell ref="A85:J85"/>
-    <mergeCell ref="K85:M85"/>
-    <mergeCell ref="N85:O85"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="A82:J82"/>
-    <mergeCell ref="K82:M82"/>
-    <mergeCell ref="N82:O82"/>
-    <mergeCell ref="P82:Q82"/>
-    <mergeCell ref="A83:J83"/>
-    <mergeCell ref="K83:M83"/>
-    <mergeCell ref="N83:O83"/>
-    <mergeCell ref="P83:Q83"/>
-    <mergeCell ref="A80:J80"/>
-    <mergeCell ref="K80:M80"/>
-    <mergeCell ref="N80:O80"/>
-    <mergeCell ref="P80:Q80"/>
-    <mergeCell ref="A81:J81"/>
-    <mergeCell ref="K81:M81"/>
-    <mergeCell ref="N81:O81"/>
-    <mergeCell ref="P81:Q81"/>
-    <mergeCell ref="A90:J90"/>
-    <mergeCell ref="K90:M90"/>
-    <mergeCell ref="N90:O90"/>
-    <mergeCell ref="P90:Q90"/>
-    <mergeCell ref="A91:J91"/>
-    <mergeCell ref="K91:M91"/>
-    <mergeCell ref="N91:O91"/>
-    <mergeCell ref="P91:Q91"/>
-    <mergeCell ref="A88:J88"/>
-    <mergeCell ref="K88:M88"/>
-    <mergeCell ref="N88:O88"/>
-    <mergeCell ref="P88:Q88"/>
-    <mergeCell ref="A89:J89"/>
-    <mergeCell ref="K89:M89"/>
-    <mergeCell ref="N89:O89"/>
-    <mergeCell ref="P89:Q89"/>
-    <mergeCell ref="A86:J86"/>
-    <mergeCell ref="K86:M86"/>
-    <mergeCell ref="N86:O86"/>
-    <mergeCell ref="P86:Q86"/>
-    <mergeCell ref="A87:J87"/>
-    <mergeCell ref="K87:M87"/>
-    <mergeCell ref="N87:O87"/>
-    <mergeCell ref="P87:Q87"/>
-    <mergeCell ref="A96:J96"/>
-    <mergeCell ref="K96:M96"/>
-    <mergeCell ref="N96:O96"/>
-    <mergeCell ref="P96:Q96"/>
-    <mergeCell ref="A97:J97"/>
-    <mergeCell ref="K97:M97"/>
-    <mergeCell ref="N97:O97"/>
-    <mergeCell ref="P97:Q97"/>
-    <mergeCell ref="A94:J94"/>
-    <mergeCell ref="K94:M94"/>
-    <mergeCell ref="N94:O94"/>
-    <mergeCell ref="P94:Q94"/>
-    <mergeCell ref="A95:J95"/>
-    <mergeCell ref="K95:M95"/>
-    <mergeCell ref="N95:O95"/>
-    <mergeCell ref="P95:Q95"/>
-    <mergeCell ref="A92:J92"/>
-    <mergeCell ref="K92:M92"/>
-    <mergeCell ref="N92:O92"/>
-    <mergeCell ref="P92:Q92"/>
-    <mergeCell ref="A93:J93"/>
-    <mergeCell ref="K93:M93"/>
-    <mergeCell ref="N93:O93"/>
-    <mergeCell ref="P93:Q93"/>
-    <mergeCell ref="A102:J102"/>
-    <mergeCell ref="K102:M102"/>
-    <mergeCell ref="N102:O102"/>
-    <mergeCell ref="P102:Q102"/>
-    <mergeCell ref="A103:J103"/>
-    <mergeCell ref="K103:M103"/>
-    <mergeCell ref="N103:O103"/>
-    <mergeCell ref="P103:Q103"/>
-    <mergeCell ref="A100:J100"/>
-    <mergeCell ref="K100:M100"/>
-    <mergeCell ref="N100:O100"/>
-    <mergeCell ref="P100:Q100"/>
-    <mergeCell ref="A101:J101"/>
-    <mergeCell ref="K101:M101"/>
-    <mergeCell ref="N101:O101"/>
-    <mergeCell ref="P101:Q101"/>
-    <mergeCell ref="A98:J98"/>
-    <mergeCell ref="K98:M98"/>
-    <mergeCell ref="N98:O98"/>
-    <mergeCell ref="P98:Q98"/>
-    <mergeCell ref="A99:J99"/>
-    <mergeCell ref="K99:M99"/>
-    <mergeCell ref="N99:O99"/>
-    <mergeCell ref="P99:Q99"/>
-    <mergeCell ref="A108:J108"/>
-    <mergeCell ref="K108:M108"/>
-    <mergeCell ref="N108:O108"/>
-    <mergeCell ref="P108:Q108"/>
-    <mergeCell ref="A109:J109"/>
-    <mergeCell ref="K109:M109"/>
-    <mergeCell ref="N109:O109"/>
-    <mergeCell ref="P109:Q109"/>
-    <mergeCell ref="A106:J106"/>
-    <mergeCell ref="K106:M106"/>
-    <mergeCell ref="N106:O106"/>
-    <mergeCell ref="P106:Q106"/>
-    <mergeCell ref="A107:J107"/>
-    <mergeCell ref="K107:M107"/>
-    <mergeCell ref="N107:O107"/>
-    <mergeCell ref="P107:Q107"/>
-    <mergeCell ref="A104:J104"/>
-    <mergeCell ref="K104:M104"/>
-    <mergeCell ref="N104:O104"/>
-    <mergeCell ref="P104:Q104"/>
-    <mergeCell ref="A105:J105"/>
-    <mergeCell ref="K105:M105"/>
-    <mergeCell ref="N105:O105"/>
-    <mergeCell ref="P105:Q105"/>
-    <mergeCell ref="A114:J114"/>
-    <mergeCell ref="K114:M114"/>
-    <mergeCell ref="N114:O114"/>
-    <mergeCell ref="P114:Q114"/>
-    <mergeCell ref="A115:J115"/>
-    <mergeCell ref="K115:M115"/>
-    <mergeCell ref="N115:O115"/>
-    <mergeCell ref="P115:Q115"/>
-    <mergeCell ref="A112:J112"/>
-    <mergeCell ref="K112:M112"/>
-    <mergeCell ref="N112:O112"/>
-    <mergeCell ref="P112:Q112"/>
-    <mergeCell ref="A113:J113"/>
-    <mergeCell ref="K113:M113"/>
-    <mergeCell ref="N113:O113"/>
-    <mergeCell ref="P113:Q113"/>
-    <mergeCell ref="A110:J110"/>
-    <mergeCell ref="K110:M110"/>
-    <mergeCell ref="N110:O110"/>
-    <mergeCell ref="P110:Q110"/>
-    <mergeCell ref="A111:J111"/>
-    <mergeCell ref="K111:M111"/>
-    <mergeCell ref="N111:O111"/>
-    <mergeCell ref="P111:Q111"/>
-    <mergeCell ref="A120:J120"/>
-    <mergeCell ref="K120:M120"/>
-    <mergeCell ref="N120:O120"/>
-    <mergeCell ref="P120:Q120"/>
-    <mergeCell ref="A121:J121"/>
-    <mergeCell ref="K121:M121"/>
-    <mergeCell ref="N121:O121"/>
-    <mergeCell ref="P121:Q121"/>
-    <mergeCell ref="A118:J118"/>
-    <mergeCell ref="K118:M118"/>
-    <mergeCell ref="N118:O118"/>
-    <mergeCell ref="P118:Q118"/>
-    <mergeCell ref="A119:J119"/>
-    <mergeCell ref="K119:M119"/>
-    <mergeCell ref="N119:O119"/>
-    <mergeCell ref="P119:Q119"/>
-    <mergeCell ref="A116:J116"/>
-    <mergeCell ref="K116:M116"/>
-    <mergeCell ref="N116:O116"/>
-    <mergeCell ref="P116:Q116"/>
-    <mergeCell ref="A117:J117"/>
-    <mergeCell ref="K117:M117"/>
-    <mergeCell ref="N117:O117"/>
-    <mergeCell ref="P117:Q117"/>
-    <mergeCell ref="A126:J126"/>
-    <mergeCell ref="K126:M126"/>
-    <mergeCell ref="N126:O126"/>
-    <mergeCell ref="P126:Q126"/>
-    <mergeCell ref="A127:J127"/>
-    <mergeCell ref="K127:M127"/>
-    <mergeCell ref="N127:O127"/>
-    <mergeCell ref="P127:Q127"/>
-    <mergeCell ref="A124:J124"/>
-    <mergeCell ref="K124:M124"/>
-    <mergeCell ref="N124:O124"/>
-    <mergeCell ref="P124:Q124"/>
-    <mergeCell ref="A125:J125"/>
-    <mergeCell ref="K125:M125"/>
-    <mergeCell ref="N125:O125"/>
-    <mergeCell ref="P125:Q125"/>
-    <mergeCell ref="A122:J122"/>
-    <mergeCell ref="K122:M122"/>
-    <mergeCell ref="N122:O122"/>
-    <mergeCell ref="P122:Q122"/>
-    <mergeCell ref="A123:J123"/>
-    <mergeCell ref="K123:M123"/>
-    <mergeCell ref="N123:O123"/>
-    <mergeCell ref="P123:Q123"/>
-    <mergeCell ref="A132:J132"/>
-    <mergeCell ref="K132:M132"/>
-    <mergeCell ref="N132:O132"/>
-    <mergeCell ref="P132:Q132"/>
-    <mergeCell ref="A133:J133"/>
-    <mergeCell ref="K133:M133"/>
-    <mergeCell ref="N133:O133"/>
-    <mergeCell ref="P133:Q133"/>
-    <mergeCell ref="A130:J130"/>
-    <mergeCell ref="K130:M130"/>
-    <mergeCell ref="N130:O130"/>
-    <mergeCell ref="P130:Q130"/>
-    <mergeCell ref="A131:J131"/>
-    <mergeCell ref="K131:M131"/>
-    <mergeCell ref="N131:O131"/>
-    <mergeCell ref="P131:Q131"/>
-    <mergeCell ref="A128:J128"/>
-    <mergeCell ref="K128:M128"/>
-    <mergeCell ref="N128:O128"/>
-    <mergeCell ref="P128:Q128"/>
-    <mergeCell ref="A129:J129"/>
-    <mergeCell ref="K129:M129"/>
-    <mergeCell ref="N129:O129"/>
-    <mergeCell ref="P129:Q129"/>
-    <mergeCell ref="A138:J138"/>
-    <mergeCell ref="K138:M138"/>
-    <mergeCell ref="N138:O138"/>
-    <mergeCell ref="P138:Q138"/>
-    <mergeCell ref="A139:J139"/>
-    <mergeCell ref="K139:M139"/>
-    <mergeCell ref="N139:O139"/>
-    <mergeCell ref="P139:Q139"/>
-    <mergeCell ref="A136:J136"/>
-    <mergeCell ref="K136:M136"/>
-    <mergeCell ref="N136:O136"/>
-    <mergeCell ref="P136:Q136"/>
-    <mergeCell ref="A137:J137"/>
-    <mergeCell ref="K137:M137"/>
-    <mergeCell ref="N137:O137"/>
-    <mergeCell ref="P137:Q137"/>
-    <mergeCell ref="A134:J134"/>
-    <mergeCell ref="K134:M134"/>
-    <mergeCell ref="N134:O134"/>
-    <mergeCell ref="P134:Q134"/>
-    <mergeCell ref="A135:J135"/>
-    <mergeCell ref="K135:M135"/>
-    <mergeCell ref="N135:O135"/>
-    <mergeCell ref="P135:Q135"/>
-    <mergeCell ref="A144:J144"/>
-    <mergeCell ref="K144:M144"/>
-    <mergeCell ref="N144:O144"/>
-    <mergeCell ref="P144:Q144"/>
-    <mergeCell ref="A145:J145"/>
-    <mergeCell ref="K145:M145"/>
-    <mergeCell ref="N145:O145"/>
-    <mergeCell ref="P145:Q145"/>
-    <mergeCell ref="A142:J142"/>
-    <mergeCell ref="K142:M142"/>
-    <mergeCell ref="N142:O142"/>
-    <mergeCell ref="P142:Q142"/>
-    <mergeCell ref="A143:J143"/>
-    <mergeCell ref="K143:M143"/>
-    <mergeCell ref="N143:O143"/>
-    <mergeCell ref="P143:Q143"/>
-    <mergeCell ref="A140:J140"/>
-    <mergeCell ref="K140:M140"/>
-    <mergeCell ref="N140:O140"/>
-    <mergeCell ref="P140:Q140"/>
-    <mergeCell ref="A141:J141"/>
-    <mergeCell ref="K141:M141"/>
-    <mergeCell ref="N141:O141"/>
-    <mergeCell ref="P141:Q141"/>
-    <mergeCell ref="A150:J150"/>
-    <mergeCell ref="K150:M150"/>
-    <mergeCell ref="N150:O150"/>
-    <mergeCell ref="P150:Q150"/>
-    <mergeCell ref="A151:J151"/>
-    <mergeCell ref="K151:M151"/>
-    <mergeCell ref="N151:O151"/>
-    <mergeCell ref="P151:Q151"/>
-    <mergeCell ref="A148:J148"/>
-    <mergeCell ref="K148:M148"/>
-    <mergeCell ref="N148:O148"/>
-    <mergeCell ref="P148:Q148"/>
-    <mergeCell ref="A149:J149"/>
-    <mergeCell ref="K149:M149"/>
-    <mergeCell ref="N149:O149"/>
-    <mergeCell ref="P149:Q149"/>
-    <mergeCell ref="A146:J146"/>
-    <mergeCell ref="K146:M146"/>
-    <mergeCell ref="N146:O146"/>
-    <mergeCell ref="P146:Q146"/>
-    <mergeCell ref="A147:J147"/>
-    <mergeCell ref="K147:M147"/>
-    <mergeCell ref="N147:O147"/>
-    <mergeCell ref="P147:Q147"/>
-    <mergeCell ref="A156:J156"/>
-    <mergeCell ref="K156:M156"/>
-    <mergeCell ref="N156:O156"/>
-    <mergeCell ref="P156:Q156"/>
-    <mergeCell ref="A157:J157"/>
-    <mergeCell ref="K157:M157"/>
-    <mergeCell ref="N157:O157"/>
-    <mergeCell ref="P157:Q157"/>
-    <mergeCell ref="A154:J154"/>
-    <mergeCell ref="K154:M154"/>
-    <mergeCell ref="N154:O154"/>
-    <mergeCell ref="P154:Q154"/>
-    <mergeCell ref="A155:J155"/>
-    <mergeCell ref="K155:M155"/>
-    <mergeCell ref="N155:O155"/>
-    <mergeCell ref="P155:Q155"/>
-    <mergeCell ref="A152:J152"/>
-    <mergeCell ref="K152:M152"/>
-    <mergeCell ref="N152:O152"/>
-    <mergeCell ref="P152:Q152"/>
-    <mergeCell ref="A153:J153"/>
-    <mergeCell ref="K153:M153"/>
-    <mergeCell ref="N153:O153"/>
-    <mergeCell ref="P153:Q153"/>
-    <mergeCell ref="A162:J162"/>
-    <mergeCell ref="K162:M162"/>
-    <mergeCell ref="N162:O162"/>
-    <mergeCell ref="P162:Q162"/>
-    <mergeCell ref="A163:J163"/>
-    <mergeCell ref="K163:M163"/>
-    <mergeCell ref="N163:O163"/>
-    <mergeCell ref="P163:Q163"/>
-    <mergeCell ref="A160:J160"/>
-    <mergeCell ref="K160:M160"/>
-    <mergeCell ref="N160:O160"/>
-    <mergeCell ref="P160:Q160"/>
-    <mergeCell ref="A161:J161"/>
-    <mergeCell ref="K161:M161"/>
-    <mergeCell ref="N161:O161"/>
-    <mergeCell ref="P161:Q161"/>
-    <mergeCell ref="A158:J158"/>
-    <mergeCell ref="K158:M158"/>
-    <mergeCell ref="N158:O158"/>
-    <mergeCell ref="P158:Q158"/>
-    <mergeCell ref="A159:J159"/>
-    <mergeCell ref="K159:M159"/>
-    <mergeCell ref="N159:O159"/>
-    <mergeCell ref="P159:Q159"/>
-    <mergeCell ref="A168:J168"/>
-    <mergeCell ref="K168:M168"/>
-    <mergeCell ref="N168:O168"/>
-    <mergeCell ref="P168:Q168"/>
-    <mergeCell ref="A169:J169"/>
-    <mergeCell ref="K169:M169"/>
-    <mergeCell ref="N169:O169"/>
-    <mergeCell ref="P169:Q169"/>
-    <mergeCell ref="A166:J166"/>
-    <mergeCell ref="K166:M166"/>
-    <mergeCell ref="N166:O166"/>
-    <mergeCell ref="P166:Q166"/>
-    <mergeCell ref="A167:J167"/>
-    <mergeCell ref="K167:M167"/>
-    <mergeCell ref="N167:O167"/>
-    <mergeCell ref="P167:Q167"/>
-    <mergeCell ref="A164:J164"/>
-    <mergeCell ref="K164:M164"/>
-    <mergeCell ref="N164:O164"/>
-    <mergeCell ref="P164:Q164"/>
-    <mergeCell ref="A165:J165"/>
-    <mergeCell ref="K165:M165"/>
-    <mergeCell ref="N165:O165"/>
-    <mergeCell ref="P165:Q165"/>
-    <mergeCell ref="A174:J174"/>
-    <mergeCell ref="K174:M174"/>
-    <mergeCell ref="N174:O174"/>
-    <mergeCell ref="P174:Q174"/>
-    <mergeCell ref="A175:J175"/>
-    <mergeCell ref="K175:M175"/>
-    <mergeCell ref="N175:O175"/>
-    <mergeCell ref="P175:Q175"/>
-    <mergeCell ref="A172:J172"/>
-    <mergeCell ref="K172:M172"/>
-    <mergeCell ref="N172:O172"/>
-    <mergeCell ref="P172:Q172"/>
-    <mergeCell ref="A173:J173"/>
-    <mergeCell ref="K173:M173"/>
-    <mergeCell ref="N173:O173"/>
-    <mergeCell ref="P173:Q173"/>
-    <mergeCell ref="A170:J170"/>
-    <mergeCell ref="K170:M170"/>
-    <mergeCell ref="N170:O170"/>
-    <mergeCell ref="P170:Q170"/>
-    <mergeCell ref="A171:J171"/>
-    <mergeCell ref="K171:M171"/>
-    <mergeCell ref="N171:O171"/>
-    <mergeCell ref="P171:Q171"/>
-    <mergeCell ref="A180:J180"/>
-    <mergeCell ref="K180:M180"/>
-    <mergeCell ref="N180:O180"/>
-    <mergeCell ref="P180:Q180"/>
-    <mergeCell ref="A181:J181"/>
-    <mergeCell ref="K181:M181"/>
-    <mergeCell ref="N181:O181"/>
-    <mergeCell ref="P181:Q181"/>
-    <mergeCell ref="A178:J178"/>
-    <mergeCell ref="K178:M178"/>
-    <mergeCell ref="N178:O178"/>
-    <mergeCell ref="P178:Q178"/>
-    <mergeCell ref="A179:J179"/>
-    <mergeCell ref="K179:M179"/>
-    <mergeCell ref="N179:O179"/>
-    <mergeCell ref="P179:Q179"/>
-    <mergeCell ref="A176:J176"/>
-    <mergeCell ref="K176:M176"/>
-    <mergeCell ref="N176:O176"/>
-    <mergeCell ref="P176:Q176"/>
-    <mergeCell ref="A177:J177"/>
-    <mergeCell ref="K177:M177"/>
-    <mergeCell ref="N177:O177"/>
-    <mergeCell ref="P177:Q177"/>
-    <mergeCell ref="A186:J186"/>
-    <mergeCell ref="K186:M186"/>
-    <mergeCell ref="N186:O186"/>
-    <mergeCell ref="P186:Q186"/>
-    <mergeCell ref="A187:J187"/>
-    <mergeCell ref="K187:M187"/>
-    <mergeCell ref="N187:O187"/>
-    <mergeCell ref="P187:Q187"/>
-    <mergeCell ref="A184:J184"/>
-    <mergeCell ref="K184:M184"/>
-    <mergeCell ref="N184:O184"/>
-    <mergeCell ref="P184:Q184"/>
-    <mergeCell ref="A185:J185"/>
-    <mergeCell ref="K185:M185"/>
-    <mergeCell ref="N185:O185"/>
-    <mergeCell ref="P185:Q185"/>
-    <mergeCell ref="A182:J182"/>
-    <mergeCell ref="K182:M182"/>
-    <mergeCell ref="N182:O182"/>
-    <mergeCell ref="P182:Q182"/>
-    <mergeCell ref="A183:J183"/>
-    <mergeCell ref="K183:M183"/>
-    <mergeCell ref="N183:O183"/>
-    <mergeCell ref="P183:Q183"/>
-    <mergeCell ref="A192:J192"/>
-    <mergeCell ref="K192:M192"/>
-    <mergeCell ref="N192:O192"/>
-    <mergeCell ref="P192:Q192"/>
-    <mergeCell ref="A193:J193"/>
-    <mergeCell ref="K193:M193"/>
-    <mergeCell ref="N193:O193"/>
-    <mergeCell ref="P193:Q193"/>
-    <mergeCell ref="A190:J190"/>
-    <mergeCell ref="K190:M190"/>
-    <mergeCell ref="N190:O190"/>
-    <mergeCell ref="P190:Q190"/>
-    <mergeCell ref="A191:J191"/>
-    <mergeCell ref="K191:M191"/>
-    <mergeCell ref="N191:O191"/>
-    <mergeCell ref="P191:Q191"/>
-    <mergeCell ref="A188:J188"/>
-    <mergeCell ref="K188:M188"/>
-    <mergeCell ref="N188:O188"/>
-    <mergeCell ref="P188:Q188"/>
-    <mergeCell ref="A189:J189"/>
-    <mergeCell ref="K189:M189"/>
-    <mergeCell ref="N189:O189"/>
-    <mergeCell ref="P189:Q189"/>
-    <mergeCell ref="A198:J198"/>
-    <mergeCell ref="K198:M198"/>
-    <mergeCell ref="N198:O198"/>
-    <mergeCell ref="P198:Q198"/>
-    <mergeCell ref="A199:J199"/>
-    <mergeCell ref="K199:M199"/>
-    <mergeCell ref="N199:O199"/>
-    <mergeCell ref="P199:Q199"/>
-    <mergeCell ref="A196:J196"/>
-    <mergeCell ref="K196:M196"/>
-    <mergeCell ref="N196:O196"/>
-    <mergeCell ref="P196:Q196"/>
-    <mergeCell ref="A197:J197"/>
-    <mergeCell ref="K197:M197"/>
-    <mergeCell ref="N197:O197"/>
-    <mergeCell ref="P197:Q197"/>
-    <mergeCell ref="A194:J194"/>
-    <mergeCell ref="K194:M194"/>
-    <mergeCell ref="N194:O194"/>
-    <mergeCell ref="P194:Q194"/>
-    <mergeCell ref="A195:J195"/>
-    <mergeCell ref="K195:M195"/>
-    <mergeCell ref="N195:O195"/>
-    <mergeCell ref="P195:Q195"/>
-    <mergeCell ref="A204:J204"/>
-    <mergeCell ref="K204:M204"/>
-    <mergeCell ref="N204:O204"/>
-    <mergeCell ref="P204:Q204"/>
-    <mergeCell ref="A205:J205"/>
-    <mergeCell ref="K205:M205"/>
-    <mergeCell ref="N205:O205"/>
-    <mergeCell ref="P205:Q205"/>
-    <mergeCell ref="A202:J202"/>
-    <mergeCell ref="K202:M202"/>
-    <mergeCell ref="N202:O202"/>
-    <mergeCell ref="P202:Q202"/>
-    <mergeCell ref="A203:J203"/>
-    <mergeCell ref="K203:M203"/>
-    <mergeCell ref="N203:O203"/>
-    <mergeCell ref="P203:Q203"/>
-    <mergeCell ref="A200:J200"/>
-    <mergeCell ref="K200:M200"/>
-    <mergeCell ref="N200:O200"/>
-    <mergeCell ref="P200:Q200"/>
-    <mergeCell ref="A201:J201"/>
-    <mergeCell ref="K201:M201"/>
-    <mergeCell ref="N201:O201"/>
-    <mergeCell ref="P201:Q201"/>
-    <mergeCell ref="A210:J210"/>
-    <mergeCell ref="K210:M210"/>
-    <mergeCell ref="N210:O210"/>
-    <mergeCell ref="P210:Q210"/>
-    <mergeCell ref="A211:J211"/>
-    <mergeCell ref="K211:M211"/>
-    <mergeCell ref="N211:O211"/>
-    <mergeCell ref="P211:Q211"/>
-    <mergeCell ref="A208:J208"/>
-    <mergeCell ref="K208:M208"/>
-    <mergeCell ref="N208:O208"/>
-    <mergeCell ref="P208:Q208"/>
-    <mergeCell ref="A209:J209"/>
-    <mergeCell ref="K209:M209"/>
-    <mergeCell ref="N209:O209"/>
-    <mergeCell ref="P209:Q209"/>
-    <mergeCell ref="A206:J206"/>
-    <mergeCell ref="K206:M206"/>
-    <mergeCell ref="N206:O206"/>
-    <mergeCell ref="P206:Q206"/>
-    <mergeCell ref="A207:J207"/>
-    <mergeCell ref="K207:M207"/>
-    <mergeCell ref="N207:O207"/>
-    <mergeCell ref="P207:Q207"/>
-    <mergeCell ref="A216:J216"/>
-    <mergeCell ref="K216:M216"/>
-    <mergeCell ref="N216:O216"/>
-    <mergeCell ref="P216:Q216"/>
-    <mergeCell ref="A217:J217"/>
-    <mergeCell ref="K217:M217"/>
-    <mergeCell ref="N217:O217"/>
-    <mergeCell ref="P217:Q217"/>
-    <mergeCell ref="A214:J214"/>
-    <mergeCell ref="K214:M214"/>
-    <mergeCell ref="N214:O214"/>
-    <mergeCell ref="P214:Q214"/>
-    <mergeCell ref="A215:J215"/>
-    <mergeCell ref="K215:M215"/>
-    <mergeCell ref="N215:O215"/>
-    <mergeCell ref="P215:Q215"/>
-    <mergeCell ref="A212:J212"/>
-    <mergeCell ref="K212:M212"/>
-    <mergeCell ref="N212:O212"/>
-    <mergeCell ref="P212:Q212"/>
-    <mergeCell ref="A213:J213"/>
-    <mergeCell ref="K213:M213"/>
-    <mergeCell ref="N213:O213"/>
-    <mergeCell ref="P213:Q213"/>
-    <mergeCell ref="A222:J222"/>
-    <mergeCell ref="K222:M222"/>
-    <mergeCell ref="N222:O222"/>
-    <mergeCell ref="P222:Q222"/>
-    <mergeCell ref="A223:J223"/>
-    <mergeCell ref="K223:M223"/>
-    <mergeCell ref="N223:O223"/>
-    <mergeCell ref="P223:Q223"/>
-    <mergeCell ref="A220:J220"/>
-    <mergeCell ref="K220:M220"/>
-    <mergeCell ref="N220:O220"/>
-    <mergeCell ref="P220:Q220"/>
-    <mergeCell ref="A221:J221"/>
-    <mergeCell ref="K221:M221"/>
-    <mergeCell ref="N221:O221"/>
-    <mergeCell ref="P221:Q221"/>
-    <mergeCell ref="A218:J218"/>
-    <mergeCell ref="K218:M218"/>
-    <mergeCell ref="N218:O218"/>
-    <mergeCell ref="P218:Q218"/>
-    <mergeCell ref="A219:J219"/>
-    <mergeCell ref="K219:M219"/>
-    <mergeCell ref="N219:O219"/>
-    <mergeCell ref="P219:Q219"/>
-    <mergeCell ref="A228:J228"/>
-    <mergeCell ref="K228:M228"/>
-    <mergeCell ref="N228:O228"/>
-    <mergeCell ref="P228:Q228"/>
-    <mergeCell ref="A229:J229"/>
-    <mergeCell ref="K229:M229"/>
-    <mergeCell ref="N229:O229"/>
-    <mergeCell ref="P229:Q229"/>
-    <mergeCell ref="A226:J226"/>
-    <mergeCell ref="K226:M226"/>
-    <mergeCell ref="N226:O226"/>
-    <mergeCell ref="P226:Q226"/>
-    <mergeCell ref="A227:J227"/>
-    <mergeCell ref="K227:M227"/>
-    <mergeCell ref="N227:O227"/>
-    <mergeCell ref="P227:Q227"/>
-    <mergeCell ref="A224:J224"/>
-    <mergeCell ref="K224:M224"/>
-    <mergeCell ref="N224:O224"/>
-    <mergeCell ref="P224:Q224"/>
-    <mergeCell ref="A225:J225"/>
-    <mergeCell ref="K225:M225"/>
-    <mergeCell ref="N225:O225"/>
-    <mergeCell ref="P225:Q225"/>
-    <mergeCell ref="A234:J234"/>
-    <mergeCell ref="K234:M234"/>
-    <mergeCell ref="N234:O234"/>
-    <mergeCell ref="P234:Q234"/>
-    <mergeCell ref="A235:J235"/>
-    <mergeCell ref="K235:M235"/>
-    <mergeCell ref="N235:O235"/>
-    <mergeCell ref="P235:Q235"/>
-    <mergeCell ref="A232:J232"/>
-    <mergeCell ref="K232:M232"/>
-    <mergeCell ref="N232:O232"/>
-    <mergeCell ref="P232:Q232"/>
-    <mergeCell ref="A233:J233"/>
-    <mergeCell ref="K233:M233"/>
-    <mergeCell ref="N233:O233"/>
-    <mergeCell ref="P233:Q233"/>
-    <mergeCell ref="A230:J230"/>
-    <mergeCell ref="K230:M230"/>
-    <mergeCell ref="N230:O230"/>
-    <mergeCell ref="P230:Q230"/>
-    <mergeCell ref="A231:J231"/>
-    <mergeCell ref="K231:M231"/>
-    <mergeCell ref="N231:O231"/>
-    <mergeCell ref="P231:Q231"/>
-    <mergeCell ref="A240:J240"/>
-    <mergeCell ref="K240:M240"/>
-    <mergeCell ref="N240:O240"/>
-    <mergeCell ref="P240:Q240"/>
-    <mergeCell ref="A241:J241"/>
-    <mergeCell ref="K241:M241"/>
-    <mergeCell ref="N241:O241"/>
-    <mergeCell ref="P241:Q241"/>
-    <mergeCell ref="A238:J238"/>
-    <mergeCell ref="K238:M238"/>
-    <mergeCell ref="N238:O238"/>
-    <mergeCell ref="P238:Q238"/>
-    <mergeCell ref="A239:J239"/>
-    <mergeCell ref="K239:M239"/>
-    <mergeCell ref="N239:O239"/>
-    <mergeCell ref="P239:Q239"/>
-    <mergeCell ref="A236:J236"/>
-    <mergeCell ref="K236:M236"/>
-    <mergeCell ref="N236:O236"/>
-    <mergeCell ref="P236:Q236"/>
-    <mergeCell ref="A237:J237"/>
-    <mergeCell ref="K237:M237"/>
-    <mergeCell ref="N237:O237"/>
-    <mergeCell ref="P237:Q237"/>
-    <mergeCell ref="A246:J246"/>
-    <mergeCell ref="K246:M246"/>
-    <mergeCell ref="N246:O246"/>
-    <mergeCell ref="P246:Q246"/>
-    <mergeCell ref="A247:J247"/>
-    <mergeCell ref="K247:M247"/>
-    <mergeCell ref="N247:O247"/>
-    <mergeCell ref="P247:Q247"/>
-    <mergeCell ref="A244:J244"/>
-    <mergeCell ref="K244:M244"/>
-    <mergeCell ref="N244:O244"/>
-    <mergeCell ref="P244:Q244"/>
-    <mergeCell ref="A245:J245"/>
-    <mergeCell ref="K245:M245"/>
-    <mergeCell ref="N245:O245"/>
-    <mergeCell ref="P245:Q245"/>
-    <mergeCell ref="A242:J242"/>
-    <mergeCell ref="K242:M242"/>
-    <mergeCell ref="N242:O242"/>
-    <mergeCell ref="P242:Q242"/>
-    <mergeCell ref="A243:J243"/>
-    <mergeCell ref="K243:M243"/>
-    <mergeCell ref="N243:O243"/>
-    <mergeCell ref="P243:Q243"/>
-    <mergeCell ref="A252:J252"/>
-    <mergeCell ref="K252:M252"/>
-    <mergeCell ref="N252:O252"/>
-    <mergeCell ref="P252:Q252"/>
-    <mergeCell ref="A253:J253"/>
-    <mergeCell ref="K253:M253"/>
-    <mergeCell ref="N253:O253"/>
-    <mergeCell ref="P253:Q253"/>
-    <mergeCell ref="A250:J250"/>
-    <mergeCell ref="K250:M250"/>
-    <mergeCell ref="N250:O250"/>
-    <mergeCell ref="P250:Q250"/>
-    <mergeCell ref="A251:J251"/>
-    <mergeCell ref="K251:M251"/>
-    <mergeCell ref="N251:O251"/>
-    <mergeCell ref="P251:Q251"/>
-    <mergeCell ref="A248:J248"/>
-    <mergeCell ref="K248:M248"/>
-    <mergeCell ref="N248:O248"/>
-    <mergeCell ref="P248:Q248"/>
-    <mergeCell ref="A249:J249"/>
-    <mergeCell ref="K249:M249"/>
-    <mergeCell ref="N249:O249"/>
-    <mergeCell ref="P249:Q249"/>
-    <mergeCell ref="A258:J258"/>
-    <mergeCell ref="K258:M258"/>
-    <mergeCell ref="N258:O258"/>
-    <mergeCell ref="P258:Q258"/>
-    <mergeCell ref="A259:J259"/>
-    <mergeCell ref="K259:M259"/>
-    <mergeCell ref="N259:O259"/>
-    <mergeCell ref="P259:Q259"/>
-    <mergeCell ref="A256:J256"/>
-    <mergeCell ref="K256:M256"/>
-    <mergeCell ref="N256:O256"/>
-    <mergeCell ref="P256:Q256"/>
-    <mergeCell ref="A257:J257"/>
-    <mergeCell ref="K257:M257"/>
-    <mergeCell ref="N257:O257"/>
-    <mergeCell ref="P257:Q257"/>
-    <mergeCell ref="A254:J254"/>
-    <mergeCell ref="K254:M254"/>
-    <mergeCell ref="N254:O254"/>
-    <mergeCell ref="P254:Q254"/>
-    <mergeCell ref="A255:J255"/>
-    <mergeCell ref="K255:M255"/>
-    <mergeCell ref="N255:O255"/>
-    <mergeCell ref="P255:Q255"/>
-    <mergeCell ref="A264:J264"/>
-    <mergeCell ref="K264:M264"/>
-    <mergeCell ref="N264:O264"/>
-    <mergeCell ref="P264:Q264"/>
-    <mergeCell ref="A265:J265"/>
-    <mergeCell ref="K265:M265"/>
-    <mergeCell ref="N265:O265"/>
-    <mergeCell ref="P265:Q265"/>
-    <mergeCell ref="A262:J262"/>
-    <mergeCell ref="K262:M262"/>
-    <mergeCell ref="N262:O262"/>
-    <mergeCell ref="P262:Q262"/>
-    <mergeCell ref="A263:J263"/>
-    <mergeCell ref="K263:M263"/>
-    <mergeCell ref="N263:O263"/>
-    <mergeCell ref="P263:Q263"/>
-    <mergeCell ref="A260:J260"/>
-    <mergeCell ref="K260:M260"/>
-    <mergeCell ref="N260:O260"/>
-    <mergeCell ref="P260:Q260"/>
-    <mergeCell ref="A261:J261"/>
-    <mergeCell ref="K261:M261"/>
-    <mergeCell ref="N261:O261"/>
-    <mergeCell ref="P261:Q261"/>
-    <mergeCell ref="A270:J270"/>
-    <mergeCell ref="K270:M270"/>
-    <mergeCell ref="N270:O270"/>
-    <mergeCell ref="P270:Q270"/>
-    <mergeCell ref="A271:J271"/>
-    <mergeCell ref="K271:M271"/>
-    <mergeCell ref="N271:O271"/>
-    <mergeCell ref="P271:Q271"/>
-    <mergeCell ref="A268:J268"/>
-    <mergeCell ref="K268:M268"/>
-    <mergeCell ref="N268:O268"/>
-    <mergeCell ref="P268:Q268"/>
-    <mergeCell ref="A269:J269"/>
-    <mergeCell ref="K269:M269"/>
-    <mergeCell ref="N269:O269"/>
-    <mergeCell ref="P269:Q269"/>
-    <mergeCell ref="A266:J266"/>
-    <mergeCell ref="K266:M266"/>
-    <mergeCell ref="N266:O266"/>
-    <mergeCell ref="P266:Q266"/>
-    <mergeCell ref="A267:J267"/>
-    <mergeCell ref="K267:M267"/>
-    <mergeCell ref="N267:O267"/>
-    <mergeCell ref="P267:Q267"/>
-    <mergeCell ref="A276:J276"/>
-    <mergeCell ref="K276:M276"/>
-    <mergeCell ref="N276:O276"/>
-    <mergeCell ref="P276:Q276"/>
-    <mergeCell ref="A277:J277"/>
-    <mergeCell ref="K277:M277"/>
-    <mergeCell ref="N277:O277"/>
-    <mergeCell ref="P277:Q277"/>
-    <mergeCell ref="A274:J274"/>
-    <mergeCell ref="K274:M274"/>
-    <mergeCell ref="N274:O274"/>
-    <mergeCell ref="P274:Q274"/>
-    <mergeCell ref="A275:J275"/>
-    <mergeCell ref="K275:M275"/>
-    <mergeCell ref="N275:O275"/>
-    <mergeCell ref="P275:Q275"/>
-    <mergeCell ref="A272:J272"/>
-    <mergeCell ref="K272:M272"/>
-    <mergeCell ref="N272:O272"/>
-    <mergeCell ref="P272:Q272"/>
-    <mergeCell ref="A273:J273"/>
-    <mergeCell ref="K273:M273"/>
-    <mergeCell ref="N273:O273"/>
-    <mergeCell ref="P273:Q273"/>
-    <mergeCell ref="A282:J282"/>
-    <mergeCell ref="K282:M282"/>
-    <mergeCell ref="N282:O282"/>
-    <mergeCell ref="P282:Q282"/>
-    <mergeCell ref="A283:J283"/>
-    <mergeCell ref="K283:M283"/>
-    <mergeCell ref="N283:O283"/>
-    <mergeCell ref="P283:Q283"/>
-    <mergeCell ref="A280:J280"/>
-    <mergeCell ref="K280:M280"/>
-    <mergeCell ref="N280:O280"/>
-    <mergeCell ref="P280:Q280"/>
-    <mergeCell ref="A281:J281"/>
-    <mergeCell ref="K281:M281"/>
-    <mergeCell ref="N281:O281"/>
-    <mergeCell ref="P281:Q281"/>
-    <mergeCell ref="A278:J278"/>
-    <mergeCell ref="K278:M278"/>
-    <mergeCell ref="N278:O278"/>
-    <mergeCell ref="P278:Q278"/>
-    <mergeCell ref="A279:J279"/>
-    <mergeCell ref="K279:M279"/>
-    <mergeCell ref="N279:O279"/>
-    <mergeCell ref="P279:Q279"/>
-    <mergeCell ref="A288:J288"/>
-    <mergeCell ref="K288:M288"/>
-    <mergeCell ref="N288:O288"/>
-    <mergeCell ref="P288:Q288"/>
-    <mergeCell ref="A289:J289"/>
-    <mergeCell ref="K289:M289"/>
-    <mergeCell ref="N289:O289"/>
-    <mergeCell ref="P289:Q289"/>
-    <mergeCell ref="A286:J286"/>
-    <mergeCell ref="K286:M286"/>
-    <mergeCell ref="N286:O286"/>
-    <mergeCell ref="P286:Q286"/>
-    <mergeCell ref="A287:J287"/>
-    <mergeCell ref="K287:M287"/>
-    <mergeCell ref="N287:O287"/>
-    <mergeCell ref="P287:Q287"/>
-    <mergeCell ref="A284:J284"/>
-    <mergeCell ref="K284:M284"/>
-    <mergeCell ref="N284:O284"/>
-    <mergeCell ref="P284:Q284"/>
-    <mergeCell ref="A285:J285"/>
-    <mergeCell ref="K285:M285"/>
-    <mergeCell ref="N285:O285"/>
-    <mergeCell ref="P285:Q285"/>
-    <mergeCell ref="A294:J294"/>
-    <mergeCell ref="K294:M294"/>
-    <mergeCell ref="N294:O294"/>
-    <mergeCell ref="P294:Q294"/>
-    <mergeCell ref="A295:J295"/>
-    <mergeCell ref="K295:M295"/>
-    <mergeCell ref="N295:O295"/>
-    <mergeCell ref="P295:Q295"/>
-    <mergeCell ref="A292:J292"/>
-    <mergeCell ref="K292:M292"/>
-    <mergeCell ref="N292:O292"/>
-    <mergeCell ref="P292:Q292"/>
-    <mergeCell ref="A293:J293"/>
-    <mergeCell ref="K293:M293"/>
-    <mergeCell ref="N293:O293"/>
-    <mergeCell ref="P293:Q293"/>
-    <mergeCell ref="A290:J290"/>
-    <mergeCell ref="K290:M290"/>
-    <mergeCell ref="N290:O290"/>
-    <mergeCell ref="P290:Q290"/>
-    <mergeCell ref="A291:J291"/>
-    <mergeCell ref="K291:M291"/>
-    <mergeCell ref="N291:O291"/>
-    <mergeCell ref="P291:Q291"/>
-    <mergeCell ref="A300:J300"/>
-    <mergeCell ref="K300:M300"/>
-    <mergeCell ref="N300:O300"/>
-    <mergeCell ref="P300:Q300"/>
-    <mergeCell ref="A301:J301"/>
-    <mergeCell ref="K301:M301"/>
-    <mergeCell ref="N301:O301"/>
-    <mergeCell ref="P301:Q301"/>
-    <mergeCell ref="A298:J298"/>
-    <mergeCell ref="K298:M298"/>
-    <mergeCell ref="N298:O298"/>
-    <mergeCell ref="P298:Q298"/>
-    <mergeCell ref="A299:J299"/>
-    <mergeCell ref="K299:M299"/>
-    <mergeCell ref="N299:O299"/>
-    <mergeCell ref="P299:Q299"/>
-    <mergeCell ref="A296:J296"/>
-    <mergeCell ref="K296:M296"/>
-    <mergeCell ref="N296:O296"/>
-    <mergeCell ref="P296:Q296"/>
-    <mergeCell ref="A297:J297"/>
-    <mergeCell ref="K297:M297"/>
-    <mergeCell ref="N297:O297"/>
-    <mergeCell ref="P297:Q297"/>
-    <mergeCell ref="A306:J306"/>
-    <mergeCell ref="K306:M306"/>
-    <mergeCell ref="N306:O306"/>
-    <mergeCell ref="P306:Q306"/>
-    <mergeCell ref="A307:J307"/>
-    <mergeCell ref="K307:M307"/>
-    <mergeCell ref="N307:O307"/>
-    <mergeCell ref="P307:Q307"/>
-    <mergeCell ref="A304:J304"/>
-    <mergeCell ref="K304:M304"/>
-    <mergeCell ref="N304:O304"/>
-    <mergeCell ref="P304:Q304"/>
-    <mergeCell ref="A305:J305"/>
-    <mergeCell ref="K305:M305"/>
-    <mergeCell ref="N305:O305"/>
-    <mergeCell ref="P305:Q305"/>
-    <mergeCell ref="A302:J302"/>
-    <mergeCell ref="K302:M302"/>
-    <mergeCell ref="N302:O302"/>
-    <mergeCell ref="P302:Q302"/>
-    <mergeCell ref="A303:J303"/>
-    <mergeCell ref="K303:M303"/>
-    <mergeCell ref="N303:O303"/>
-    <mergeCell ref="P303:Q303"/>
-    <mergeCell ref="A312:J312"/>
-    <mergeCell ref="K312:M312"/>
-    <mergeCell ref="N312:O312"/>
-    <mergeCell ref="P312:Q312"/>
-    <mergeCell ref="A313:J313"/>
-    <mergeCell ref="K313:M313"/>
-    <mergeCell ref="N313:O313"/>
-    <mergeCell ref="P313:Q313"/>
-    <mergeCell ref="A310:J310"/>
-    <mergeCell ref="K310:M310"/>
-    <mergeCell ref="N310:O310"/>
-    <mergeCell ref="P310:Q310"/>
-    <mergeCell ref="A311:J311"/>
-    <mergeCell ref="K311:M311"/>
-    <mergeCell ref="N311:O311"/>
-    <mergeCell ref="P311:Q311"/>
-    <mergeCell ref="A308:J308"/>
-    <mergeCell ref="K308:M308"/>
-    <mergeCell ref="N308:O308"/>
-    <mergeCell ref="P308:Q308"/>
-    <mergeCell ref="A309:J309"/>
-    <mergeCell ref="K309:M309"/>
-    <mergeCell ref="N309:O309"/>
-    <mergeCell ref="P309:Q309"/>
-    <mergeCell ref="A318:J318"/>
-    <mergeCell ref="K318:M318"/>
-    <mergeCell ref="N318:O318"/>
-    <mergeCell ref="P318:Q318"/>
-    <mergeCell ref="A319:J319"/>
-    <mergeCell ref="K319:M319"/>
-    <mergeCell ref="N319:O319"/>
-    <mergeCell ref="P319:Q319"/>
-    <mergeCell ref="A316:J316"/>
-    <mergeCell ref="K316:M316"/>
-    <mergeCell ref="N316:O316"/>
-    <mergeCell ref="P316:Q316"/>
-    <mergeCell ref="A317:J317"/>
-    <mergeCell ref="K317:M317"/>
-    <mergeCell ref="N317:O317"/>
-    <mergeCell ref="P317:Q317"/>
-    <mergeCell ref="A314:J314"/>
-    <mergeCell ref="K314:M314"/>
-    <mergeCell ref="N314:O314"/>
-    <mergeCell ref="P314:Q314"/>
-    <mergeCell ref="A315:J315"/>
-    <mergeCell ref="K315:M315"/>
-    <mergeCell ref="N315:O315"/>
-    <mergeCell ref="P315:Q315"/>
-    <mergeCell ref="A324:J324"/>
-    <mergeCell ref="K324:M324"/>
-    <mergeCell ref="N324:O324"/>
-    <mergeCell ref="P324:Q324"/>
-    <mergeCell ref="A325:J325"/>
-    <mergeCell ref="K325:M325"/>
-    <mergeCell ref="N325:O325"/>
-    <mergeCell ref="P325:Q325"/>
-    <mergeCell ref="A322:J322"/>
-    <mergeCell ref="K322:M322"/>
-    <mergeCell ref="N322:O322"/>
-    <mergeCell ref="P322:Q322"/>
-    <mergeCell ref="A323:J323"/>
-    <mergeCell ref="K323:M323"/>
-    <mergeCell ref="N323:O323"/>
-    <mergeCell ref="P323:Q323"/>
-    <mergeCell ref="A320:J320"/>
-    <mergeCell ref="K320:M320"/>
-    <mergeCell ref="N320:O320"/>
-    <mergeCell ref="P320:Q320"/>
-    <mergeCell ref="A321:J321"/>
-    <mergeCell ref="K321:M321"/>
-    <mergeCell ref="N321:O321"/>
-    <mergeCell ref="P321:Q321"/>
-    <mergeCell ref="A330:J330"/>
-    <mergeCell ref="K330:M330"/>
-    <mergeCell ref="N330:O330"/>
-    <mergeCell ref="P330:Q330"/>
-    <mergeCell ref="A331:J331"/>
-    <mergeCell ref="K331:M331"/>
-    <mergeCell ref="N331:O331"/>
-    <mergeCell ref="P331:Q331"/>
-    <mergeCell ref="A328:J328"/>
-    <mergeCell ref="K328:M328"/>
-    <mergeCell ref="N328:O328"/>
-    <mergeCell ref="P328:Q328"/>
-    <mergeCell ref="A329:J329"/>
-    <mergeCell ref="K329:M329"/>
-    <mergeCell ref="N329:O329"/>
-    <mergeCell ref="P329:Q329"/>
-    <mergeCell ref="A326:J326"/>
-    <mergeCell ref="K326:M326"/>
-    <mergeCell ref="N326:O326"/>
-    <mergeCell ref="P326:Q326"/>
-    <mergeCell ref="A327:J327"/>
-    <mergeCell ref="K327:M327"/>
-    <mergeCell ref="N327:O327"/>
-    <mergeCell ref="P327:Q327"/>
-    <mergeCell ref="A336:J336"/>
-    <mergeCell ref="K336:M336"/>
-    <mergeCell ref="N336:O336"/>
-    <mergeCell ref="P336:Q336"/>
-    <mergeCell ref="A337:J337"/>
-    <mergeCell ref="K337:M337"/>
-    <mergeCell ref="N337:O337"/>
-    <mergeCell ref="P337:Q337"/>
-    <mergeCell ref="A334:J334"/>
-    <mergeCell ref="K334:M334"/>
-    <mergeCell ref="N334:O334"/>
-    <mergeCell ref="P334:Q334"/>
-    <mergeCell ref="A335:J335"/>
-    <mergeCell ref="K335:M335"/>
-    <mergeCell ref="N335:O335"/>
-    <mergeCell ref="P335:Q335"/>
-    <mergeCell ref="A332:J332"/>
-    <mergeCell ref="K332:M332"/>
-    <mergeCell ref="N332:O332"/>
-    <mergeCell ref="P332:Q332"/>
-    <mergeCell ref="A333:J333"/>
-    <mergeCell ref="K333:M333"/>
-    <mergeCell ref="N333:O333"/>
-    <mergeCell ref="P333:Q333"/>
-    <mergeCell ref="A342:J342"/>
-    <mergeCell ref="K342:M342"/>
-    <mergeCell ref="N342:O342"/>
-    <mergeCell ref="P342:Q342"/>
-    <mergeCell ref="A343:J343"/>
-    <mergeCell ref="K343:M343"/>
-    <mergeCell ref="N343:O343"/>
-    <mergeCell ref="P343:Q343"/>
-    <mergeCell ref="A340:J340"/>
-    <mergeCell ref="K340:M340"/>
-    <mergeCell ref="N340:O340"/>
-    <mergeCell ref="P340:Q340"/>
-    <mergeCell ref="A341:J341"/>
-    <mergeCell ref="K341:M341"/>
-    <mergeCell ref="N341:O341"/>
-    <mergeCell ref="P341:Q341"/>
-    <mergeCell ref="A338:J338"/>
-    <mergeCell ref="K338:M338"/>
-    <mergeCell ref="N338:O338"/>
-    <mergeCell ref="P338:Q338"/>
-    <mergeCell ref="A339:J339"/>
-    <mergeCell ref="K339:M339"/>
-    <mergeCell ref="N339:O339"/>
-    <mergeCell ref="P339:Q339"/>
-    <mergeCell ref="A348:J348"/>
-    <mergeCell ref="K348:M348"/>
-    <mergeCell ref="N348:O348"/>
-    <mergeCell ref="P348:Q348"/>
-    <mergeCell ref="A349:J349"/>
-    <mergeCell ref="K349:M349"/>
-    <mergeCell ref="N349:O349"/>
-    <mergeCell ref="P349:Q349"/>
-    <mergeCell ref="A346:J346"/>
-    <mergeCell ref="K346:M346"/>
-    <mergeCell ref="N346:O346"/>
-    <mergeCell ref="P346:Q346"/>
-    <mergeCell ref="A347:J347"/>
-    <mergeCell ref="K347:M347"/>
-    <mergeCell ref="N347:O347"/>
-    <mergeCell ref="P347:Q347"/>
-    <mergeCell ref="A344:J344"/>
-    <mergeCell ref="K344:M344"/>
-    <mergeCell ref="N344:O344"/>
-    <mergeCell ref="P344:Q344"/>
-    <mergeCell ref="A345:J345"/>
-    <mergeCell ref="K345:M345"/>
-    <mergeCell ref="N345:O345"/>
-    <mergeCell ref="P345:Q345"/>
-    <mergeCell ref="A354:J354"/>
-    <mergeCell ref="K354:M354"/>
-    <mergeCell ref="N354:O354"/>
-    <mergeCell ref="P354:Q354"/>
-    <mergeCell ref="A355:J355"/>
-    <mergeCell ref="K355:M355"/>
-    <mergeCell ref="N355:O355"/>
-    <mergeCell ref="P355:Q355"/>
-    <mergeCell ref="A352:J352"/>
-    <mergeCell ref="K352:M352"/>
-    <mergeCell ref="N352:O352"/>
-    <mergeCell ref="P352:Q352"/>
-    <mergeCell ref="A353:J353"/>
-    <mergeCell ref="K353:M353"/>
-    <mergeCell ref="N353:O353"/>
-    <mergeCell ref="P353:Q353"/>
-    <mergeCell ref="A350:J350"/>
-    <mergeCell ref="K350:M350"/>
-    <mergeCell ref="N350:O350"/>
-    <mergeCell ref="P350:Q350"/>
-    <mergeCell ref="A351:J351"/>
-    <mergeCell ref="K351:M351"/>
-    <mergeCell ref="N351:O351"/>
-    <mergeCell ref="P351:Q351"/>
-    <mergeCell ref="A360:J360"/>
-    <mergeCell ref="K360:M360"/>
-    <mergeCell ref="N360:O360"/>
-    <mergeCell ref="P360:Q360"/>
-    <mergeCell ref="A361:J361"/>
-    <mergeCell ref="K361:M361"/>
-    <mergeCell ref="N361:O361"/>
-    <mergeCell ref="P361:Q361"/>
-    <mergeCell ref="A358:J358"/>
-    <mergeCell ref="K358:M358"/>
-    <mergeCell ref="N358:O358"/>
-    <mergeCell ref="P358:Q358"/>
-    <mergeCell ref="A359:J359"/>
-    <mergeCell ref="K359:M359"/>
-    <mergeCell ref="N359:O359"/>
-    <mergeCell ref="P359:Q359"/>
-    <mergeCell ref="A356:J356"/>
-    <mergeCell ref="K356:M356"/>
-    <mergeCell ref="N356:O356"/>
-    <mergeCell ref="P356:Q356"/>
-    <mergeCell ref="A357:J357"/>
-    <mergeCell ref="K357:M357"/>
-    <mergeCell ref="N357:O357"/>
-    <mergeCell ref="P357:Q357"/>
-    <mergeCell ref="A366:J366"/>
-    <mergeCell ref="K366:M366"/>
-    <mergeCell ref="N366:O366"/>
-    <mergeCell ref="P366:Q366"/>
-    <mergeCell ref="A367:J367"/>
-    <mergeCell ref="K367:M367"/>
-    <mergeCell ref="N367:O367"/>
-    <mergeCell ref="P367:Q367"/>
-    <mergeCell ref="A364:J364"/>
-    <mergeCell ref="K364:M364"/>
-    <mergeCell ref="N364:O364"/>
-    <mergeCell ref="P364:Q364"/>
-    <mergeCell ref="A365:J365"/>
-    <mergeCell ref="K365:M365"/>
-    <mergeCell ref="N365:O365"/>
-    <mergeCell ref="P365:Q365"/>
-    <mergeCell ref="A362:J362"/>
-    <mergeCell ref="K362:M362"/>
-    <mergeCell ref="N362:O362"/>
-    <mergeCell ref="P362:Q362"/>
-    <mergeCell ref="A363:J363"/>
-    <mergeCell ref="K363:M363"/>
-    <mergeCell ref="N363:O363"/>
-    <mergeCell ref="P363:Q363"/>
-    <mergeCell ref="A372:J372"/>
-    <mergeCell ref="K372:M372"/>
-    <mergeCell ref="N372:O372"/>
-    <mergeCell ref="P372:Q372"/>
-    <mergeCell ref="A373:J373"/>
-    <mergeCell ref="K373:M373"/>
-    <mergeCell ref="N373:O373"/>
-    <mergeCell ref="P373:Q373"/>
-    <mergeCell ref="A370:J370"/>
-    <mergeCell ref="K370:M370"/>
-    <mergeCell ref="N370:O370"/>
-    <mergeCell ref="P370:Q370"/>
-    <mergeCell ref="A371:J371"/>
-    <mergeCell ref="K371:M371"/>
-    <mergeCell ref="N371:O371"/>
-    <mergeCell ref="P371:Q371"/>
-    <mergeCell ref="A368:J368"/>
-    <mergeCell ref="K368:M368"/>
-    <mergeCell ref="N368:O368"/>
-    <mergeCell ref="P368:Q368"/>
-    <mergeCell ref="A369:J369"/>
-    <mergeCell ref="K369:M369"/>
-    <mergeCell ref="N369:O369"/>
-    <mergeCell ref="P369:Q369"/>
-    <mergeCell ref="A378:J378"/>
-    <mergeCell ref="K378:M378"/>
-    <mergeCell ref="N378:O378"/>
-    <mergeCell ref="P378:Q378"/>
-    <mergeCell ref="A379:J379"/>
-    <mergeCell ref="K379:M379"/>
-    <mergeCell ref="N379:O379"/>
-    <mergeCell ref="P379:Q379"/>
-    <mergeCell ref="A376:J376"/>
-    <mergeCell ref="K376:M376"/>
-    <mergeCell ref="N376:O376"/>
-    <mergeCell ref="P376:Q376"/>
-    <mergeCell ref="A377:J377"/>
-    <mergeCell ref="K377:M377"/>
-    <mergeCell ref="N377:O377"/>
-    <mergeCell ref="P377:Q377"/>
-    <mergeCell ref="A374:J374"/>
-    <mergeCell ref="K374:M374"/>
-    <mergeCell ref="N374:O374"/>
-    <mergeCell ref="P374:Q374"/>
-    <mergeCell ref="A375:J375"/>
-    <mergeCell ref="K375:M375"/>
-    <mergeCell ref="N375:O375"/>
-    <mergeCell ref="P375:Q375"/>
-    <mergeCell ref="A384:J384"/>
-    <mergeCell ref="K384:M384"/>
-    <mergeCell ref="N384:O384"/>
-    <mergeCell ref="P384:Q384"/>
-    <mergeCell ref="A385:J385"/>
-    <mergeCell ref="K385:M385"/>
-    <mergeCell ref="N385:O385"/>
-    <mergeCell ref="P385:Q385"/>
-    <mergeCell ref="A382:J382"/>
-    <mergeCell ref="K382:M382"/>
-    <mergeCell ref="N382:O382"/>
-    <mergeCell ref="P382:Q382"/>
-    <mergeCell ref="A383:J383"/>
-    <mergeCell ref="K383:M383"/>
-    <mergeCell ref="N383:O383"/>
-    <mergeCell ref="P383:Q383"/>
-    <mergeCell ref="A380:J380"/>
-    <mergeCell ref="K380:M380"/>
-    <mergeCell ref="N380:O380"/>
-    <mergeCell ref="P380:Q380"/>
-    <mergeCell ref="A381:J381"/>
-    <mergeCell ref="K381:M381"/>
-    <mergeCell ref="N381:O381"/>
-    <mergeCell ref="P381:Q381"/>
-    <mergeCell ref="A390:J390"/>
-    <mergeCell ref="K390:M390"/>
-    <mergeCell ref="N390:O390"/>
-    <mergeCell ref="P390:Q390"/>
-    <mergeCell ref="A391:J391"/>
-    <mergeCell ref="K391:M391"/>
-    <mergeCell ref="N391:O391"/>
-    <mergeCell ref="P391:Q391"/>
-    <mergeCell ref="A388:J388"/>
-    <mergeCell ref="K388:M388"/>
-    <mergeCell ref="N388:O388"/>
-    <mergeCell ref="P388:Q388"/>
-    <mergeCell ref="A389:J389"/>
-    <mergeCell ref="K389:M389"/>
-    <mergeCell ref="N389:O389"/>
-    <mergeCell ref="P389:Q389"/>
-    <mergeCell ref="A386:J386"/>
-    <mergeCell ref="K386:M386"/>
-    <mergeCell ref="N386:O386"/>
-    <mergeCell ref="P386:Q386"/>
-    <mergeCell ref="A387:J387"/>
-    <mergeCell ref="K387:M387"/>
-    <mergeCell ref="N387:O387"/>
-    <mergeCell ref="P387:Q387"/>
-    <mergeCell ref="A396:J396"/>
-    <mergeCell ref="K396:M396"/>
-    <mergeCell ref="N396:O396"/>
-    <mergeCell ref="P396:Q396"/>
-    <mergeCell ref="A397:J397"/>
-    <mergeCell ref="K397:M397"/>
-    <mergeCell ref="N397:O397"/>
-    <mergeCell ref="P397:Q397"/>
-    <mergeCell ref="A394:J394"/>
-    <mergeCell ref="K394:M394"/>
-    <mergeCell ref="N394:O394"/>
-    <mergeCell ref="P394:Q394"/>
-    <mergeCell ref="A395:J395"/>
-    <mergeCell ref="K395:M395"/>
-    <mergeCell ref="N395:O395"/>
-    <mergeCell ref="P395:Q395"/>
-    <mergeCell ref="A392:J392"/>
-    <mergeCell ref="K392:M392"/>
-    <mergeCell ref="N392:O392"/>
-    <mergeCell ref="P392:Q392"/>
-    <mergeCell ref="A393:J393"/>
-    <mergeCell ref="K393:M393"/>
-    <mergeCell ref="N393:O393"/>
-    <mergeCell ref="P393:Q393"/>
-    <mergeCell ref="A402:J402"/>
-    <mergeCell ref="K402:M402"/>
-    <mergeCell ref="N402:O402"/>
-    <mergeCell ref="P402:Q402"/>
-    <mergeCell ref="A403:J403"/>
-    <mergeCell ref="K403:M403"/>
-    <mergeCell ref="N403:O403"/>
-    <mergeCell ref="P403:Q403"/>
-    <mergeCell ref="A400:J400"/>
-    <mergeCell ref="K400:M400"/>
-    <mergeCell ref="N400:O400"/>
-    <mergeCell ref="P400:Q400"/>
-    <mergeCell ref="A401:J401"/>
-    <mergeCell ref="K401:M401"/>
-    <mergeCell ref="N401:O401"/>
-    <mergeCell ref="P401:Q401"/>
-    <mergeCell ref="A398:J398"/>
-    <mergeCell ref="K398:M398"/>
-    <mergeCell ref="N398:O398"/>
-    <mergeCell ref="P398:Q398"/>
-    <mergeCell ref="A399:J399"/>
-    <mergeCell ref="K399:M399"/>
-    <mergeCell ref="N399:O399"/>
-    <mergeCell ref="P399:Q399"/>
-    <mergeCell ref="A408:J408"/>
-    <mergeCell ref="K408:M408"/>
-    <mergeCell ref="N408:O408"/>
-    <mergeCell ref="P408:Q408"/>
-    <mergeCell ref="A409:J409"/>
-    <mergeCell ref="K409:M409"/>
-    <mergeCell ref="N409:O409"/>
-    <mergeCell ref="P409:Q409"/>
-    <mergeCell ref="A406:J406"/>
-    <mergeCell ref="K406:M406"/>
-    <mergeCell ref="N406:O406"/>
-    <mergeCell ref="P406:Q406"/>
-    <mergeCell ref="A407:J407"/>
-    <mergeCell ref="K407:M407"/>
-    <mergeCell ref="N407:O407"/>
-    <mergeCell ref="P407:Q407"/>
-    <mergeCell ref="A404:J404"/>
-    <mergeCell ref="K404:M404"/>
-    <mergeCell ref="N404:O404"/>
-    <mergeCell ref="P404:Q404"/>
-    <mergeCell ref="A405:J405"/>
-    <mergeCell ref="K405:M405"/>
-    <mergeCell ref="N405:O405"/>
-    <mergeCell ref="P405:Q405"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="A1:Z5"/>
+    <mergeCell ref="A6:Z8"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:Q9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Divide Two Integers
</commit_message>
<xml_diff>
--- a/LeetCode_Results.xlsx
+++ b/LeetCode_Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>LeetCode Practice Results</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>String to Integer (atoi)</t>
+  </si>
+  <si>
+    <t>Divide Two Integers</t>
   </si>
 </sst>
 </file>
@@ -741,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23:Q23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +895,7 @@
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="str">
         <f>"Average Results: " &amp; "Faster than "  &amp; ROUNDDOWN(AVERAGE(N10:O500), 2) &amp; "% and has less memory usage over " &amp; ROUNDDOWN(AVERAGE(P10:Q500), 2) &amp; "% out of all C# submissions."</f>
-        <v>Average Results: Faster than 89.25% and has less memory usage over 43.08% out of all C# submissions.</v>
+        <v>Average Results: Faster than 89.98% and has less memory usage over 47.14% out of all C# submissions.</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -1102,7 +1105,7 @@
       <c r="Q12" s="2"/>
       <c r="S12" s="24" t="str">
         <f>"Medium: " &amp; SUMPRODUCT((LEN(K10:M500)-LEN(SUBSTITUTE(K10:M500,"Medium","")))/LEN("Medium"))</f>
-        <v>Medium: 2</v>
+        <v>Medium: 3</v>
       </c>
       <c r="T12" s="24"/>
       <c r="U12" s="24"/>
@@ -1271,7 +1274,7 @@
       <c r="Q17" s="2"/>
       <c r="S17" s="26" t="str">
         <f>COUNTA(A10:J500) &amp; " problems answered"</f>
-        <v>13 problems answered</v>
+        <v>14 problems answered</v>
       </c>
       <c r="T17" s="27"/>
       <c r="U17" s="27"/>
@@ -1430,7 +1433,9 @@
       <c r="Q22" s="2"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
+      <c r="A23" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1440,12 +1445,18 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="2"/>
+      <c r="K23" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
-      <c r="N23" s="3"/>
+      <c r="N23" s="3">
+        <v>99.43</v>
+      </c>
       <c r="O23" s="3"/>
-      <c r="P23" s="2"/>
+      <c r="P23" s="2">
+        <v>100</v>
+      </c>
       <c r="Q23" s="2"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>